<commit_message>
minor update to user used
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C71B50-7414-47A7-9FA4-2622459CC51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3D69E9-0630-4DD5-B811-9EDFE0CFB0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25635" yWindow="1200" windowWidth="23925" windowHeight="18165" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="12045" yWindow="3225" windowWidth="23925" windowHeight="14430" activeTab="1" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -138,10 +138,6 @@
   </si>
   <si>
     <t>Tested against a Pi 3 running Buster, with the user wxcapture.
-If using a different username, you will need to modify paths, crontab info, etc.</t>
-  </si>
-  <si>
-    <t>Tested against a VirtualBox VM running Debian x, with the user wxcapture.
 If using a different username, you will need to modify paths, crontab info, etc.</t>
   </si>
   <si>
@@ -1143,6 +1139,10 @@
   </si>
   <si>
     <t>autospawn=yes</t>
+  </si>
+  <si>
+    <t>Tested against a VirtualBox VM running Debian x, with the user mike
+If using a different username, you will need to modify paths, crontab info, etc.</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
   <dimension ref="A1:C233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -1634,7 +1634,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1662,61 +1662,61 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
@@ -1829,52 +1829,52 @@
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1882,78 +1882,78 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1961,40 +1961,40 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2002,34 +2002,34 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,40 +2037,40 @@
     </row>
     <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2078,50 +2078,50 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2129,70 +2129,70 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2201,166 +2201,166 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C114" t="s">
         <v>133</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C114" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C115" s="4"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C119" s="4"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C120" s="4"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C121" s="4"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C122" s="4"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C123" s="4"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C126" s="4"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C127" s="4"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C128" s="4"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C129" s="4"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C130" s="4"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C131" s="4"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C133" s="4"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C134" s="4"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C135" s="4"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
       <c r="B136" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C136" s="4"/>
     </row>
@@ -2370,482 +2370,482 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>62</v>
+      </c>
+      <c r="B150" t="s">
         <v>63</v>
-      </c>
-      <c r="B150" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>65</v>
+      </c>
+      <c r="B154" t="s">
         <v>66</v>
-      </c>
-      <c r="B154" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B162" t="s">
         <v>101</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
         <v>102</v>
-      </c>
-      <c r="C162" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B165" t="s">
         <v>105</v>
-      </c>
-      <c r="B165" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B168" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C168" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B169" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>151</v>
+      </c>
+      <c r="B171" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B171" s="10" t="s">
-        <v>153</v>
-      </c>
       <c r="C171" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>159</v>
+      </c>
+      <c r="B174" t="s">
         <v>160</v>
-      </c>
-      <c r="B174" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>161</v>
+      </c>
+      <c r="B176" t="s">
         <v>162</v>
-      </c>
-      <c r="B176" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C178" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
+        <v>165</v>
+      </c>
+      <c r="C179" t="s">
         <v>166</v>
-      </c>
-      <c r="C179" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B181" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C182" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
+        <v>165</v>
+      </c>
+      <c r="C183" t="s">
         <v>166</v>
-      </c>
-      <c r="C183" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>170</v>
+      </c>
+      <c r="B187" t="s">
         <v>171</v>
       </c>
-      <c r="B187" t="s">
-        <v>172</v>
-      </c>
       <c r="C187" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
+        <v>172</v>
+      </c>
+      <c r="C188" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="C188" s="9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B190" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C190" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>179</v>
+      </c>
+      <c r="B192" t="s">
         <v>180</v>
-      </c>
-      <c r="B192" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>185</v>
+      </c>
+      <c r="B197" t="s">
         <v>186</v>
-      </c>
-      <c r="B197" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
+        <v>187</v>
+      </c>
+      <c r="C198" t="s">
         <v>188</v>
-      </c>
-      <c r="C198" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B200" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B202" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B207" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B210" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B211" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B212" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B213" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C213" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B215" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
+        <v>222</v>
+      </c>
+      <c r="C216" t="s">
         <v>223</v>
-      </c>
-      <c r="C216" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B218" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B219" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B220" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>144</v>
+      </c>
+      <c r="B224" t="s">
         <v>145</v>
       </c>
-      <c r="B224" t="s">
-        <v>146</v>
-      </c>
       <c r="C224" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C225" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
+        <v>153</v>
+      </c>
+      <c r="B230" t="s">
         <v>154</v>
-      </c>
-      <c r="B230" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="B231" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="330" x14ac:dyDescent="0.25">
       <c r="B233" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2861,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD9A0C4-7338-415A-8AC4-B66EAEFEBD21}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,7 +2877,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>35</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -2886,17 +2886,17 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -2952,12 +2952,12 @@
         <v>17</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2967,183 +2967,183 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
-      </c>
-      <c r="B33" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="B44" t="s">
-        <v>213</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>234</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>244</v>
+      </c>
+      <c r="B54" t="s">
         <v>245</v>
-      </c>
-      <c r="B54" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3157,7 +3157,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3172,7 +3172,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>35</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -3181,24 +3181,24 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C5" s="7"/>
     </row>
@@ -3215,38 +3215,38 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
receive_morse code - #26
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6617FDC8-2D18-42BD-9D09-7CBA92CC254F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AF7A6A-09AA-41AA-B7AB-A2B98C389579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1290" windowWidth="23925" windowHeight="18780" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="19515" yWindow="1365" windowWidth="30045" windowHeight="16200" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="267">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -1107,6 +1107,27 @@
   <si>
     <t>Tested against a VirtualBox VM running Debian 10, with the user mike
 If using a different username, you will need to modify paths, crontab info, etc.</t>
+  </si>
+  <si>
+    <t>install multimon-ng</t>
+  </si>
+  <si>
+    <t>cd ~/temp</t>
+  </si>
+  <si>
+    <t>git clone git://github.com/EliasOenal/multimon-ng.git</t>
+  </si>
+  <si>
+    <t>cd multimon-ng</t>
+  </si>
+  <si>
+    <t>mkdir build</t>
+  </si>
+  <si>
+    <t>cd build</t>
+  </si>
+  <si>
+    <t>qmake ../multimon-ng.pro</t>
   </si>
 </sst>
 </file>
@@ -1541,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,488 +2275,550 @@
       <c r="C121" s="4"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C122" s="4"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="4"/>
+      <c r="B123" t="s">
+        <v>262</v>
+      </c>
+      <c r="C123" s="4"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="4"/>
+      <c r="B124" t="s">
+        <v>263</v>
+      </c>
+      <c r="C124" s="4"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="4"/>
+      <c r="B125" t="s">
+        <v>264</v>
+      </c>
+      <c r="C125" s="4"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="4"/>
+      <c r="B126" t="s">
+        <v>265</v>
+      </c>
+      <c r="C126" s="4"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="4"/>
+      <c r="B127" t="s">
+        <v>266</v>
+      </c>
+      <c r="C127" s="4"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="4"/>
+      <c r="B128" t="s">
+        <v>77</v>
+      </c>
+      <c r="C128" s="4"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="4"/>
+      <c r="B129" t="s">
+        <v>78</v>
+      </c>
+      <c r="C129" s="4"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="4"/>
+      <c r="C130" s="4"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>50</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>60</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>62</v>
-      </c>
       <c r="B134" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>65</v>
-      </c>
       <c r="B138" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="4" t="s">
-        <v>90</v>
+      <c r="A143" t="s">
+        <v>62</v>
       </c>
       <c r="B143" t="s">
-        <v>91</v>
-      </c>
-      <c r="C143" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B146" t="s">
-        <v>95</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="4"/>
+      <c r="A147" t="s">
+        <v>65</v>
+      </c>
       <c r="B147" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="4"/>
       <c r="B148" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C149" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B150" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>100</v>
+      <c r="B149" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>138</v>
-      </c>
-      <c r="B152" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C152" s="11" t="s">
-        <v>162</v>
+      <c r="A152" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B152" t="s">
+        <v>91</v>
+      </c>
+      <c r="C152" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B155" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="4"/>
+      <c r="B156" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+      <c r="B157" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C158" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B159" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>138</v>
+      </c>
+      <c r="B161" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C161" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>146</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B164" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>148</v>
-      </c>
-      <c r="B157" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>151</v>
-      </c>
-      <c r="C159" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>152</v>
-      </c>
-      <c r="C160" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>154</v>
-      </c>
-      <c r="B162" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>151</v>
-      </c>
-      <c r="C163" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
-        <v>152</v>
-      </c>
-      <c r="C164" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B166" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>157</v>
-      </c>
       <c r="B168" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C168" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>159</v>
-      </c>
-      <c r="C169" s="9" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="C169" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>154</v>
+      </c>
+      <c r="B171" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>151</v>
+      </c>
+      <c r="C172" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>152</v>
+      </c>
+      <c r="C173" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>155</v>
+      </c>
+      <c r="B175" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>157</v>
+      </c>
+      <c r="B177" t="s">
+        <v>158</v>
+      </c>
+      <c r="C177" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>159</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>156</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B180" t="s">
         <v>161</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C180" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>166</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B182" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>172</v>
-      </c>
-      <c r="B178" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>174</v>
-      </c>
-      <c r="C179" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>171</v>
-      </c>
-      <c r="B181" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>177</v>
-      </c>
-      <c r="B183" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>172</v>
+      </c>
+      <c r="B187" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
+        <v>174</v>
+      </c>
+      <c r="C188" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>171</v>
+      </c>
+      <c r="B190" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>177</v>
+      </c>
+      <c r="B192" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>182</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B197" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B190" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B191" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B192" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B193" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B194" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C194" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B196" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>209</v>
-      </c>
-      <c r="C197" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B199" s="4" t="s">
-        <v>188</v>
+      <c r="B199" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" s="4" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="4" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B202" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
-        <v>211</v>
-      </c>
-      <c r="C203" s="4" t="s">
-        <v>215</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B203" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C203" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>131</v>
-      </c>
-      <c r="B205" t="s">
-        <v>132</v>
-      </c>
-      <c r="C205" t="s">
-        <v>136</v>
+      <c r="B205" s="4" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>133</v>
+        <v>209</v>
       </c>
       <c r="C206" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B208" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B209" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B210" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B211" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>211</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>131</v>
+      </c>
+      <c r="B214" t="s">
+        <v>132</v>
+      </c>
+      <c r="C214" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>133</v>
+      </c>
+      <c r="C215" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B208" t="s">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>140</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B220" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="B212" s="4" t="s">
+    <row r="221" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B221" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="B214" s="4" t="s">
+    <row r="223" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="B223" s="4" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C169" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
+    <hyperlink ref="C178" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
satellites page and misc improvements
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AF7A6A-09AA-41AA-B7AB-A2B98C389579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831646C6-95CE-4E0F-A249-20BEDA4B2E4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19515" yWindow="1365" windowWidth="30045" windowHeight="16200" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="13185" yWindow="525" windowWidth="25080" windowHeight="20565" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="266">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -777,9 +777,6 @@
   </si>
   <si>
     <t>if not using Discord, set discord webooks to no</t>
-  </si>
-  <si>
-    <t>can only use Discord if also using Twitter as twitter URL for the images are used</t>
   </si>
   <si>
     <t>config-METEOR.json</t>
@@ -1564,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
   <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,154 +2116,154 @@
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C99" s="4"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C100" s="4"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C101" s="4"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C102" s="4"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C103" s="4"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C104" s="4"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C105" s="4"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C106" s="4"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C107" s="4"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C108" s="4"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C109" s="4"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C110" s="4"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C111" s="4"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C112" s="4"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C113" s="4"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C114" s="4"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C115" s="4"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C119" s="4"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C120" s="4"/>
     </row>
@@ -2276,45 +2273,45 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>261</v>
       </c>
       <c r="C122" s="4"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C123" s="4"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C126" s="4"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C127" s="4"/>
     </row>
@@ -2495,7 +2492,7 @@
         <v>139</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2529,7 +2526,7 @@
         <v>151</v>
       </c>
       <c r="C168" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2537,12 +2534,12 @@
         <v>152</v>
       </c>
       <c r="C169" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B171" t="s">
         <v>147</v>
@@ -2553,7 +2550,7 @@
         <v>151</v>
       </c>
       <c r="C172" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,12 +2558,12 @@
         <v>152</v>
       </c>
       <c r="C173" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B175" t="s">
         <v>147</v>
@@ -2574,107 +2571,107 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>156</v>
+      </c>
+      <c r="B177" t="s">
         <v>157</v>
       </c>
-      <c r="B177" t="s">
-        <v>158</v>
-      </c>
       <c r="C177" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
+        <v>158</v>
+      </c>
+      <c r="C178" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="C178" s="9" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B180" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C180" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>165</v>
+      </c>
+      <c r="B182" t="s">
         <v>166</v>
-      </c>
-      <c r="B182" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>171</v>
+      </c>
+      <c r="B187" t="s">
         <v>172</v>
-      </c>
-      <c r="B187" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
+        <v>173</v>
+      </c>
+      <c r="C188" t="s">
         <v>174</v>
-      </c>
-      <c r="C188" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B190" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B192" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B197" t="s">
         <v>79</v>
@@ -2682,81 +2679,81 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B202" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B203" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C203" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B205" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
+        <v>208</v>
+      </c>
+      <c r="C206" t="s">
         <v>209</v>
-      </c>
-      <c r="C206" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B209" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B210" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B211" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -2845,7 +2842,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -2864,14 +2861,14 @@
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -2932,7 +2929,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2942,7 +2939,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2957,7 +2954,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2990,17 +2987,17 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3023,7 +3020,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B37" t="s">
         <v>66</v>
@@ -3031,94 +3028,94 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44" t="s">
+        <v>198</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="B44" t="s">
-        <v>199</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>221</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>230</v>
+      </c>
+      <c r="B54" t="s">
         <v>231</v>
-      </c>
-      <c r="B54" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3144,10 +3141,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -3166,20 +3163,20 @@
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3198,7 +3195,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9" t="s">
         <v>66</v>
@@ -3206,22 +3203,22 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
@@ -3229,7 +3226,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates based on user feedback
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831646C6-95CE-4E0F-A249-20BEDA4B2E4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152858E4-993D-4CBA-B612-C362D506D45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13185" yWindow="525" windowWidth="25080" windowHeight="20565" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="22290" yWindow="1455" windowWidth="28440" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="268">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -334,14 +334,6 @@
   </si>
   <si>
     <t>Add the following:</t>
-  </si>
-  <si>
-    <t>Update the following fields:
-Registration email:
-Ground Station:
-Latitude:
-Longitude:
-Altitude:</t>
   </si>
   <si>
     <t>Install Meteor-M2 Demodulator</t>
@@ -1125,6 +1117,22 @@
   </si>
   <si>
     <t>qmake ../multimon-ng.pro</t>
+  </si>
+  <si>
+    <t>sudo apt-get install python3-pip</t>
+  </si>
+  <si>
+    <t>Only need to do this section if you do not have a pi user already set up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+click into the cell, select all the content, copy, paste and you'll see the file in nano be well formatted, as it appears here
+Update the following fields:
+Registration email:
+Ground Station:
+Latitude:
+Longitude:
+Altitude:</t>
   </si>
 </sst>
 </file>
@@ -1559,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,10 +1655,10 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1658,13 +1666,16 @@
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
+      <c r="C15" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1706,1116 +1717,1121 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-    </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
+      <c r="B63" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
-    </row>
-    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="B69" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
+      <c r="B76" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
       <c r="B81" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
-      <c r="B82" s="4" t="s">
-        <v>107</v>
+      <c r="B82" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
+      <c r="B85" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B86" s="4" t="s">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="B97" s="4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C99" t="s">
         <v>122</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C98" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C99" s="4"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C100" s="4"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
-      <c r="B101" t="s">
-        <v>234</v>
+      <c r="B101" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="C101" s="4"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C102" s="4"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C103" s="4"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C104" s="4"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C105" s="4"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C106" s="4"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C107" s="4"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C108" s="4"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C109" s="4"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C110" s="4"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C111" s="4"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C112" s="4"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C113" s="4"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C114" s="4"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C115" s="4"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C119" s="4"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C120" s="4"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
+      <c r="B121" t="s">
+        <v>254</v>
+      </c>
       <c r="C121" s="4"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="4"/>
+      <c r="C122" s="4"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>259</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="C122" s="4"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
-      <c r="B123" t="s">
-        <v>261</v>
       </c>
       <c r="C123" s="4"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C126" s="4"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C127" s="4"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" t="s">
-        <v>77</v>
+        <v>264</v>
       </c>
       <c r="C128" s="4"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C129" s="4"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
+      <c r="B130" t="s">
+        <v>78</v>
+      </c>
       <c r="C130" s="4"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="4"/>
+      <c r="C131" s="4"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>50</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>62</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B144" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>65</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B153" t="s">
         <v>91</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C153" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="4" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B156" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="4"/>
-      <c r="B156" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="4"/>
+      <c r="B158" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B158" s="4" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B159" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C159" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B159" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="160" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>137</v>
+      </c>
+      <c r="B162" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B161" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C161" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="C162" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>145</v>
+      </c>
+      <c r="B165" t="s">
         <v>146</v>
       </c>
-      <c r="B164" t="s">
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="B167" t="s">
         <v>148</v>
-      </c>
-      <c r="B166" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B167" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>151</v>
-      </c>
-      <c r="C168" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
+        <v>150</v>
+      </c>
+      <c r="C169" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>151</v>
+      </c>
+      <c r="C170" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>152</v>
       </c>
-      <c r="C169" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>153</v>
-      </c>
-      <c r="B171" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>151</v>
-      </c>
-      <c r="C172" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C173" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>151</v>
+      </c>
+      <c r="C174" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>153</v>
+      </c>
+      <c r="B176" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>155</v>
+      </c>
+      <c r="B178" t="s">
+        <v>156</v>
+      </c>
+      <c r="C178" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>157</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>154</v>
       </c>
-      <c r="B175" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>156</v>
-      </c>
-      <c r="B177" t="s">
-        <v>157</v>
-      </c>
-      <c r="C177" t="s">
+      <c r="B181" t="s">
+        <v>159</v>
+      </c>
+      <c r="C181" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>158</v>
-      </c>
-      <c r="C178" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>155</v>
-      </c>
-      <c r="B180" t="s">
-        <v>160</v>
-      </c>
-      <c r="C180" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="B183" t="s">
         <v>165</v>
-      </c>
-      <c r="B182" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>170</v>
+      </c>
+      <c r="B188" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>172</v>
+      </c>
+      <c r="C189" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>171</v>
-      </c>
-      <c r="B187" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
-        <v>173</v>
-      </c>
-      <c r="C188" t="s">
+      <c r="B191" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>170</v>
-      </c>
-      <c r="B190" t="s">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>176</v>
-      </c>
-      <c r="B192" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>181</v>
-      </c>
-      <c r="B197" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>180</v>
+      </c>
+      <c r="B198" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B200" s="4" t="s">
-        <v>184</v>
+      <c r="B200" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B202" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B203" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C203" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B205" s="4" t="s">
-        <v>207</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B204" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C204" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
-        <v>208</v>
-      </c>
-      <c r="C206" t="s">
-        <v>209</v>
+      <c r="B206" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>210</v>
+        <v>207</v>
+      </c>
+      <c r="C207" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B208" s="4" t="s">
-        <v>187</v>
+      <c r="B208" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B209" s="4" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B210" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B211" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B212" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>209</v>
+      </c>
+      <c r="C213" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
-        <v>210</v>
-      </c>
-      <c r="C212" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>130</v>
+      </c>
+      <c r="B215" t="s">
         <v>131</v>
       </c>
-      <c r="B214" t="s">
-        <v>132</v>
-      </c>
-      <c r="C214" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B215" t="s">
-        <v>133</v>
-      </c>
       <c r="C215" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+      <c r="C216" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>139</v>
+      </c>
+      <c r="B221" t="s">
         <v>140</v>
       </c>
-      <c r="B220" t="s">
+    </row>
+    <row r="222" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B222" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B221" s="4" t="s">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B222" t="s">
+    <row r="224" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="B224" s="4" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="330" x14ac:dyDescent="0.25">
-      <c r="B223" s="4" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C178" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
+    <hyperlink ref="C179" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -2842,7 +2858,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -2861,14 +2877,14 @@
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -2929,7 +2945,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2939,7 +2955,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2954,7 +2970,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2987,17 +3003,17 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3020,7 +3036,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B37" t="s">
         <v>66</v>
@@ -3028,94 +3044,94 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B44" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B44" t="s">
-        <v>198</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>220</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" t="s">
         <v>230</v>
-      </c>
-      <c r="B54" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3141,10 +3157,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -3163,20 +3179,20 @@
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3195,7 +3211,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" t="s">
         <v>66</v>
@@ -3203,22 +3219,22 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
@@ -3226,7 +3242,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
noaa image height capture, additional instructions
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152858E4-993D-4CBA-B612-C362D506D45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DB43C3-9191-41D4-A6CD-1CACC34A732B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22290" yWindow="1455" windowWidth="28440" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="22635" yWindow="1800" windowWidth="28440" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="268">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -1569,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
   <dimension ref="A1:C224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2840,10 +2840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD9A0C4-7338-415A-8AC4-B66EAEFEBD21}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,202 +2935,208 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B16" s="12" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>33</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>190</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>193</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>198</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>197</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>219</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B53" s="14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>229</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>232</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates from alpha testing
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DB43C3-9191-41D4-A6CD-1CACC34A732B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C732EC-3980-42F7-BA9D-05C1197B2F7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22635" yWindow="1800" windowWidth="28440" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="29310" yWindow="1875" windowWidth="22350" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="275">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -732,6 +732,397 @@
     <t>Add to the end:</t>
   </si>
   <si>
+    <t>Note, config needs to be updated</t>
+  </si>
+  <si>
+    <t>config-AMSAT.json</t>
+  </si>
+  <si>
+    <t>use gain values as a good starting point, can adjust up / down</t>
+  </si>
+  <si>
+    <t>config-NOAA.json</t>
+  </si>
+  <si>
+    <t>update branding text</t>
+  </si>
+  <si>
+    <t>Key config to validate is as listed</t>
+  </si>
+  <si>
+    <t>if not tweeting, set tweet to no</t>
+  </si>
+  <si>
+    <t>if not using Discord, set discord webooks to no</t>
+  </si>
+  <si>
+    <t>config-METEOR.json</t>
+  </si>
+  <si>
+    <t>config-SSTV.json</t>
+  </si>
+  <si>
+    <t>config-discord.json</t>
+  </si>
+  <si>
+    <t>config-twitter.json</t>
+  </si>
+  <si>
+    <t>set up all values to reflect your Twitter account</t>
+  </si>
+  <si>
+    <t>this account must have access to the Twitter API to get most of the values</t>
+  </si>
+  <si>
+    <t>https://developer.twitter.com/en/apply-for-access</t>
+  </si>
+  <si>
+    <t>set up all values to reflect your Discord account</t>
+  </si>
+  <si>
+    <t>There needs to be a full configuration document built</t>
+  </si>
+  <si>
+    <t>recommend not using Twitter / Discord when first starting</t>
+  </si>
+  <si>
+    <t>recommend not using Twitter when first starting</t>
+  </si>
+  <si>
+    <t>recommend not using Discord when first starting</t>
+  </si>
+  <si>
+    <t>config.json</t>
+  </si>
+  <si>
+    <t>update the following fields</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>GPS location NS</t>
+  </si>
+  <si>
+    <t>GPS location EW</t>
+  </si>
+  <si>
+    <t>satellites.json</t>
+  </si>
+  <si>
+    <t>sdr.json</t>
+  </si>
+  <si>
+    <t>Update to reflect your SDR</t>
+  </si>
+  <si>
+    <t>serial number is vital as this is how the SDR is selected</t>
+  </si>
+  <si>
+    <t>To change serial numbers for an SDR - http://www.cloud-sdr.com/tutorial-sharing-two-rtlsdr-receivers/</t>
+  </si>
+  <si>
+    <t>ensure the sdr value matches that in sdr.json</t>
+  </si>
+  <si>
+    <t>config-rsync.json</t>
+  </si>
+  <si>
+    <t>remote user</t>
+  </si>
+  <si>
+    <t>remote directory</t>
+  </si>
+  <si>
+    <t>remote host</t>
+  </si>
+  <si>
+    <t>set the following values to reflect the server used to host the website</t>
+  </si>
+  <si>
+    <t>set up key for rsync</t>
+  </si>
+  <si>
+    <t>mkdir .ssh</t>
+  </si>
+  <si>
+    <t>cd .ssh</t>
+  </si>
+  <si>
+    <t>ssh-keygen -t rsa</t>
+  </si>
+  <si>
+    <t>press enter when prompted</t>
+  </si>
+  <si>
+    <t>double enter for passphrase</t>
+  </si>
+  <si>
+    <t>cd .ssh/</t>
+  </si>
+  <si>
+    <t>At this point you need to have the server set up for the website - pause here until you have at least the fixed IP address and the username you will use, with the server up and running</t>
+  </si>
+  <si>
+    <t>This server must have a fixed IP address, which you will need to set up yourself.</t>
+  </si>
+  <si>
+    <t>Suggest performing the Server tab setup and then returning here</t>
+  </si>
+  <si>
+    <t>mkdir wxcapture/web</t>
+  </si>
+  <si>
+    <t>mkdir wxcapture/web/logs</t>
+  </si>
+  <si>
+    <t>mkdir wxcapture/web/config</t>
+  </si>
+  <si>
+    <t>move server files</t>
+  </si>
+  <si>
+    <t>cp -r git_source/wxcapture/server-code/wxcapture/web/* wxcapture/web/</t>
+  </si>
+  <si>
+    <t>chmod +x wxcapture/web/*.py</t>
+  </si>
+  <si>
+    <t>sudo apt install apache2</t>
+  </si>
+  <si>
+    <t>grep -i mike *</t>
+  </si>
+  <si>
+    <t>Update user</t>
+  </si>
+  <si>
+    <t>if using a user other than mike, identify where the code has a directory path which includes mike and update to reflect the user used</t>
+  </si>
+  <si>
+    <t>config_server.py</t>
+  </si>
+  <si>
+    <t>fix_pass_pages_lib.py</t>
+  </si>
+  <si>
+    <t>fix_pass_pages.py</t>
+  </si>
+  <si>
+    <t>meteor_pages.py</t>
+  </si>
+  <si>
+    <t>move_modal.py</t>
+  </si>
+  <si>
+    <t>noaa_pages.py</t>
+  </si>
+  <si>
+    <t>copy to server</t>
+  </si>
+  <si>
+    <t>scp id_rsa.pub mike@192.168.x.x:/home/mike/.ssh</t>
+  </si>
+  <si>
+    <t>update mike and IP address to reflect your server user / IP</t>
+  </si>
+  <si>
+    <t>ssh mike@192.168.x.x</t>
+  </si>
+  <si>
+    <t>mv id_rsa.pub authorized_keys</t>
+  </si>
+  <si>
+    <t>chmod 700 authorized_keys</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>should not need a password</t>
+  </si>
+  <si>
+    <t>sudo apt install python3-pip</t>
+  </si>
+  <si>
+    <t>cp git_source/wxcapture/pi-code/wxcapture/process/wxcutils.py wxcapture/web/</t>
+  </si>
+  <si>
+    <t>cp git_source/wxcapture/pi-code/wxcapture/process/config/*.txt wxcapture/web/config/</t>
+  </si>
+  <si>
+    <t>sudo pip3 install python-dateutil</t>
+  </si>
+  <si>
+    <t>cp git_source/wxcapture/pi-code/wxcapture/process/config/satellites.json wxcapture/web/config/</t>
+  </si>
+  <si>
+    <t>Website set up</t>
+  </si>
+  <si>
+    <t>Complete the set up in the Website Tab, then return here</t>
+  </si>
+  <si>
+    <t>This write up assumes the server is the same sever as the website server</t>
+  </si>
+  <si>
+    <t>move website files</t>
+  </si>
+  <si>
+    <t>sudo cp -r git_source/wxcapture/server-website/wxcapture/* /var/www/html/</t>
+  </si>
+  <si>
+    <t>install lightbox</t>
+  </si>
+  <si>
+    <t>git clone https://github.com/lokesh/lightbox2</t>
+  </si>
+  <si>
+    <t>sudo mkdir /var/www/html/lightbox</t>
+  </si>
+  <si>
+    <t>sudo cp -r lightbox2/dist/* /var/www/html/lightbox/</t>
+  </si>
+  <si>
+    <t>It assumes that Apache2 is installed and the document root is /var/www/html/</t>
+  </si>
+  <si>
+    <t>setup scheduled jobs</t>
+  </si>
+  <si>
+    <t>sudo crontab -e</t>
+  </si>
+  <si>
+    <t>append to the end of the file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Run the file move script every 2 minutes
+*/2 * * * * /home/mike/wxcapture/web/move_modal.py &gt; /dev/null 2&gt;&amp;1
+# Run the meteor page script at 4 minutes after midnight
+4 0 * * * /home/mike/wxcapture/web/meteor_pages.py &gt; /dev/null 2&gt;&amp;1
+# Run the noaa page script at 4 minutes after midnight
+4 0 * * * /home/mike/wxcapture/web/noaa_pages.py &gt; /dev/null 2&gt;&amp;1
+# Run the config validation script - 1 minute past midnight
+1 0 * * *  /home/mike/wxcapture/web/config_server.py  &gt; /dev/null 2&gt;&amp;1
+</t>
+  </si>
+  <si>
+    <t>output tab - ensure that the "null output" shows</t>
+  </si>
+  <si>
+    <t>recording tab - ensure that QSSTV is set to monitor Null Output</t>
+  </si>
+  <si>
+    <t>qsstv &amp;</t>
+  </si>
+  <si>
+    <t>pavucontrol &amp;</t>
+  </si>
+  <si>
+    <t>close pavucontrol - X on the window!</t>
+  </si>
+  <si>
+    <t>In QSSTV</t>
+  </si>
+  <si>
+    <t>ensure that Auto Slant and Autosave are set</t>
+  </si>
+  <si>
+    <t>Options -&gt; configuration &gt; Sound tab</t>
+  </si>
+  <si>
+    <t>ensure that:</t>
+  </si>
+  <si>
+    <t>the Input Audio Device and the Output Audio Device are set to "pulse -- PulseAudio Sound Server"</t>
+  </si>
+  <si>
+    <t>Sound input = From sound card</t>
+  </si>
+  <si>
+    <t>Sound output = To sound card</t>
+  </si>
+  <si>
+    <t>Audio interface - PulseAudio</t>
+  </si>
+  <si>
+    <t>Directories tab</t>
+  </si>
+  <si>
+    <t>set RX SSTV Images to /home/pi/wxcapture/process/working/</t>
+  </si>
+  <si>
+    <t>OK to save</t>
+  </si>
+  <si>
+    <t>exit QSSTV</t>
+  </si>
+  <si>
+    <t>sudo nano /etc/pulse/client.conf.d/00-disable-autospawn.conf</t>
+  </si>
+  <si>
+    <t>change:</t>
+  </si>
+  <si>
+    <t>autospawn=no</t>
+  </si>
+  <si>
+    <t>to:</t>
+  </si>
+  <si>
+    <t>autospawn=yes</t>
+  </si>
+  <si>
+    <t>The code will write pages to the webserver document root, unless otherwise configured. If you have existing website content, take a backup.</t>
+  </si>
+  <si>
+    <t>WxCapture - Setup Website</t>
+  </si>
+  <si>
+    <t>Tested against a VirtualBox VM running Debian 10, with the user mike
+If using a different username, you will need to modify paths, crontab info, etc.</t>
+  </si>
+  <si>
+    <t>install multimon-ng</t>
+  </si>
+  <si>
+    <t>cd ~/temp</t>
+  </si>
+  <si>
+    <t>git clone git://github.com/EliasOenal/multimon-ng.git</t>
+  </si>
+  <si>
+    <t>cd multimon-ng</t>
+  </si>
+  <si>
+    <t>mkdir build</t>
+  </si>
+  <si>
+    <t>cd build</t>
+  </si>
+  <si>
+    <t>qmake ../multimon-ng.pro</t>
+  </si>
+  <si>
+    <t>sudo apt-get install python3-pip</t>
+  </si>
+  <si>
+    <t>Only need to do this section if you do not have a pi user already set up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+click into the cell, select all the content, copy, paste and you'll see the file in nano be well formatted, as it appears here
+Update the following fields:
+Registration email:
+Ground Station:
+Latitude:
+Longitude:
+Altitude:</t>
+  </si>
+  <si>
+    <t>sudo apt-get install python-matplotlib</t>
+  </si>
+  <si>
     <t xml:space="preserve"># run the weather satellite prediction code - v2
 # run at 3 minutes past midnight each night OR after a reboot
 3 0 * * * export DISPLAY=:0.0 &amp;&amp; 3 0 * * * DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
@@ -742,397 +1133,29 @@
 1 0 * * *  /home/pi/wxcapture/process/update_planets_tle.py  &gt; /dev/null 2&gt;&amp;1
 # update Satellite Status - 1 minute past midnight
 1 0 * * *  /home/pi/wxcapture/process/satellite_status.py  &gt; /dev/null 2&gt;&amp;1
+# Run the file sync script every 2 minutes on every odd minute
+1-59/2 * * * * /home/pi/wxcapture/process/sync.py &gt; /dev/null 2&gt;&amp;1
 # Run the config validation script - 1 minute past midnight
 1 0 * * *  /home/pi/wxcapture/process/config.py  &gt; /dev/null 2&gt;&amp;1
 </t>
   </si>
   <si>
-    <t>Note, config needs to be updated</t>
-  </si>
-  <si>
-    <t>config-AMSAT.json</t>
-  </si>
-  <si>
-    <t>use gain values as a good starting point, can adjust up / down</t>
-  </si>
-  <si>
-    <t>config-NOAA.json</t>
-  </si>
-  <si>
-    <t>update branding text</t>
-  </si>
-  <si>
-    <t>Key config to validate is as listed</t>
-  </si>
-  <si>
-    <t>if not tweeting, set tweet to no</t>
-  </si>
-  <si>
-    <t>if not using Discord, set discord webooks to no</t>
-  </si>
-  <si>
-    <t>config-METEOR.json</t>
-  </si>
-  <si>
-    <t>config-SSTV.json</t>
-  </si>
-  <si>
-    <t>config-discord.json</t>
-  </si>
-  <si>
-    <t>config-twitter.json</t>
-  </si>
-  <si>
-    <t>set up all values to reflect your Twitter account</t>
-  </si>
-  <si>
-    <t>this account must have access to the Twitter API to get most of the values</t>
-  </si>
-  <si>
-    <t>https://developer.twitter.com/en/apply-for-access</t>
-  </si>
-  <si>
-    <t>set up all values to reflect your Discord account</t>
-  </si>
-  <si>
-    <t>There needs to be a full configuration document built</t>
-  </si>
-  <si>
-    <t>recommend not using Twitter / Discord when first starting</t>
-  </si>
-  <si>
-    <t>recommend not using Twitter when first starting</t>
-  </si>
-  <si>
-    <t>recommend not using Discord when first starting</t>
-  </si>
-  <si>
-    <t>config.json</t>
-  </si>
-  <si>
-    <t>update the following fields</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>GPS location NS</t>
-  </si>
-  <si>
-    <t>GPS location EW</t>
-  </si>
-  <si>
-    <t>satellites.json</t>
-  </si>
-  <si>
-    <t>sdr.json</t>
-  </si>
-  <si>
-    <t>Update to reflect your SDR</t>
-  </si>
-  <si>
-    <t>serial number is vital as this is how the SDR is selected</t>
-  </si>
-  <si>
-    <t>To change serial numbers for an SDR - http://www.cloud-sdr.com/tutorial-sharing-two-rtlsdr-receivers/</t>
-  </si>
-  <si>
-    <t>ensure the sdr value matches that in sdr.json</t>
-  </si>
-  <si>
-    <t>config-rsync.json</t>
-  </si>
-  <si>
-    <t>remote user</t>
-  </si>
-  <si>
-    <t>remote directory</t>
-  </si>
-  <si>
-    <t>remote host</t>
-  </si>
-  <si>
-    <t>set the following values to reflect the server used to host the website</t>
-  </si>
-  <si>
-    <t>set up key for rsync</t>
-  </si>
-  <si>
-    <t>mkdir .ssh</t>
-  </si>
-  <si>
-    <t>cd .ssh</t>
-  </si>
-  <si>
-    <t>ssh-keygen -t rsa</t>
-  </si>
-  <si>
-    <t>press enter when prompted</t>
-  </si>
-  <si>
-    <t>double enter for passphrase</t>
-  </si>
-  <si>
-    <t>cd .ssh/</t>
-  </si>
-  <si>
-    <t>At this point you need to have the server set up for the website - pause here until you have at least the fixed IP address and the username you will use, with the server up and running</t>
-  </si>
-  <si>
-    <t>This server must have a fixed IP address, which you will need to set up yourself.</t>
-  </si>
-  <si>
-    <t>Suggest performing the Server tab setup and then returning here</t>
-  </si>
-  <si>
-    <t>mkdir wxcapture/web</t>
-  </si>
-  <si>
-    <t>mkdir wxcapture/web/logs</t>
-  </si>
-  <si>
-    <t>mkdir wxcapture/web/config</t>
-  </si>
-  <si>
-    <t>move server files</t>
-  </si>
-  <si>
-    <t>cp -r git_source/wxcapture/server-code/wxcapture/web/* wxcapture/web/</t>
-  </si>
-  <si>
-    <t>chmod +x wxcapture/web/*.py</t>
-  </si>
-  <si>
-    <t>sudo apt install apache2</t>
-  </si>
-  <si>
-    <t>grep -i mike *</t>
-  </si>
-  <si>
-    <t>Update user</t>
-  </si>
-  <si>
-    <t>if using a user other than mike, identify where the code has a directory path which includes mike and update to reflect the user used</t>
-  </si>
-  <si>
-    <t>config_server.py</t>
-  </si>
-  <si>
-    <t>fix_pass_pages_lib.py</t>
-  </si>
-  <si>
-    <t>fix_pass_pages.py</t>
-  </si>
-  <si>
-    <t>meteor_pages.py</t>
-  </si>
-  <si>
-    <t>move_modal.py</t>
-  </si>
-  <si>
-    <t>noaa_pages.py</t>
-  </si>
-  <si>
-    <t>copy to server</t>
-  </si>
-  <si>
-    <t>scp id_rsa.pub mike@192.168.x.x:/home/mike/.ssh</t>
-  </si>
-  <si>
-    <t>update mike and IP address to reflect your server user / IP</t>
-  </si>
-  <si>
-    <t>ssh mike@192.168.x.x</t>
-  </si>
-  <si>
-    <t>mv id_rsa.pub authorized_keys</t>
-  </si>
-  <si>
-    <t>chmod 700 authorized_keys</t>
-  </si>
-  <si>
-    <t>exit</t>
-  </si>
-  <si>
-    <t>should not need a password</t>
-  </si>
-  <si>
-    <t>sudo apt install python3-pip</t>
-  </si>
-  <si>
-    <t>cp git_source/wxcapture/pi-code/wxcapture/process/wxcutils.py wxcapture/web/</t>
-  </si>
-  <si>
-    <t>cp git_source/wxcapture/pi-code/wxcapture/process/config/*.txt wxcapture/web/config/</t>
-  </si>
-  <si>
-    <t>sudo pip3 install python-dateutil</t>
-  </si>
-  <si>
-    <t>cp git_source/wxcapture/pi-code/wxcapture/process/config/satellites.json wxcapture/web/config/</t>
-  </si>
-  <si>
-    <t>Website set up</t>
-  </si>
-  <si>
-    <t>Complete the set up in the Website Tab, then return here</t>
-  </si>
-  <si>
-    <t>This write up assumes the server is the same sever as the website server</t>
-  </si>
-  <si>
-    <t>move website files</t>
-  </si>
-  <si>
-    <t>sudo cp -r git_source/wxcapture/server-website/wxcapture/* /var/www/html/</t>
-  </si>
-  <si>
-    <t>install lightbox</t>
-  </si>
-  <si>
-    <t>git clone https://github.com/lokesh/lightbox2</t>
-  </si>
-  <si>
-    <t>sudo mkdir /var/www/html/lightbox</t>
-  </si>
-  <si>
-    <t>sudo cp -r lightbox2/dist/* /var/www/html/lightbox/</t>
-  </si>
-  <si>
-    <t>It assumes that Apache2 is installed and the document root is /var/www/html/</t>
-  </si>
-  <si>
-    <t>setup scheduled jobs</t>
-  </si>
-  <si>
-    <t>sudo crontab -e</t>
-  </si>
-  <si>
-    <t>append to the end of the file</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Run the file move script every 2 minutes
-*/2 * * * * /home/mike/wxcapture/web/move_modal.py &gt; /dev/null 2&gt;&amp;1
-# Run the meteor page script at 4 minutes after midnight
-4 0 * * * /home/mike/wxcapture/web/meteor_pages.py &gt; /dev/null 2&gt;&amp;1
-# Run the noaa page script at 4 minutes after midnight
-4 0 * * * /home/mike/wxcapture/web/noaa_pages.py &gt; /dev/null 2&gt;&amp;1
-# Run the config validation script - 1 minute past midnight
-1 0 * * *  /home/mike/wxcapture/web/config_server.py  &gt; /dev/null 2&gt;&amp;1
-</t>
-  </si>
-  <si>
-    <t>output tab - ensure that the "null output" shows</t>
-  </si>
-  <si>
-    <t>recording tab - ensure that QSSTV is set to monitor Null Output</t>
-  </si>
-  <si>
-    <t>qsstv &amp;</t>
-  </si>
-  <si>
-    <t>pavucontrol &amp;</t>
-  </si>
-  <si>
-    <t>close pavucontrol - X on the window!</t>
-  </si>
-  <si>
-    <t>In QSSTV</t>
-  </si>
-  <si>
-    <t>ensure that Auto Slant and Autosave are set</t>
-  </si>
-  <si>
-    <t>Options -&gt; configuration &gt; Sound tab</t>
-  </si>
-  <si>
-    <t>ensure that:</t>
-  </si>
-  <si>
-    <t>the Input Audio Device and the Output Audio Device are set to "pulse -- PulseAudio Sound Server"</t>
-  </si>
-  <si>
-    <t>Sound input = From sound card</t>
-  </si>
-  <si>
-    <t>Sound output = To sound card</t>
-  </si>
-  <si>
-    <t>Audio interface - PulseAudio</t>
-  </si>
-  <si>
-    <t>Directories tab</t>
-  </si>
-  <si>
-    <t>set RX SSTV Images to /home/pi/wxcapture/process/working/</t>
-  </si>
-  <si>
-    <t>OK to save</t>
-  </si>
-  <si>
-    <t>exit QSSTV</t>
-  </si>
-  <si>
-    <t>sudo nano /etc/pulse/client.conf.d/00-disable-autospawn.conf</t>
-  </si>
-  <si>
-    <t>change:</t>
-  </si>
-  <si>
-    <t>autospawn=no</t>
-  </si>
-  <si>
-    <t>to:</t>
-  </si>
-  <si>
-    <t>autospawn=yes</t>
-  </si>
-  <si>
-    <t>The code will write pages to the webserver document root, unless otherwise configured. If you have existing website content, take a backup.</t>
-  </si>
-  <si>
-    <t>WxCapture - Setup Website</t>
-  </si>
-  <si>
-    <t>Tested against a VirtualBox VM running Debian 10, with the user mike
-If using a different username, you will need to modify paths, crontab info, etc.</t>
-  </si>
-  <si>
-    <t>install multimon-ng</t>
-  </si>
-  <si>
-    <t>cd ~/temp</t>
-  </si>
-  <si>
-    <t>git clone git://github.com/EliasOenal/multimon-ng.git</t>
-  </si>
-  <si>
-    <t>cd multimon-ng</t>
-  </si>
-  <si>
-    <t>mkdir build</t>
-  </si>
-  <si>
-    <t>cd build</t>
-  </si>
-  <si>
-    <t>qmake ../multimon-ng.pro</t>
-  </si>
-  <si>
-    <t>sudo apt-get install python3-pip</t>
-  </si>
-  <si>
-    <t>Only need to do this section if you do not have a pi user already set up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-click into the cell, select all the content, copy, paste and you'll see the file in nano be well formatted, as it appears here
-Update the following fields:
-Registration email:
-Ground Station:
-Latitude:
-Longitude:
-Altitude:</t>
+    <t>Update config</t>
+  </si>
+  <si>
+    <t>cd wxcapture/web/config</t>
+  </si>
+  <si>
+    <t>nano config.json</t>
+  </si>
+  <si>
+    <t>look for the line which includes:</t>
+  </si>
+  <si>
+    <t>"web doc root location": "/home/websites/wxcapture/",</t>
+  </si>
+  <si>
+    <t>change the directory in the second set of "" to show where you have the website set up - i.e. where index.html, etc. are</t>
   </si>
 </sst>
 </file>
@@ -1567,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,7 +1681,7 @@
         <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,7 +1740,7 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1835,1003 +1858,1008 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
-        <v>69</v>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-    </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
-    </row>
-    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="B70" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
-      <c r="B83" s="4" t="s">
-        <v>106</v>
+      <c r="B83" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
+      <c r="B86" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="B98" s="4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="C100" s="4"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C101" s="4"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
-      <c r="B102" t="s">
-        <v>233</v>
+      <c r="B102" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="C102" s="4"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C103" s="4"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C104" s="4"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C105" s="4"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C106" s="4"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C107" s="4"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C108" s="4"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C109" s="4"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C110" s="4"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C111" s="4"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C112" s="4"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C113" s="4"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C114" s="4"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C115" s="4"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C119" s="4"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C120" s="4"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C121" s="4"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
+      <c r="B122" t="s">
+        <v>253</v>
+      </c>
       <c r="C122" s="4"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="4"/>
+      <c r="C123" s="4"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B124" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C123" s="4"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
-      <c r="B124" t="s">
-        <v>260</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C126" s="4"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C127" s="4"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C128" s="4"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" t="s">
-        <v>77</v>
+        <v>263</v>
       </c>
       <c r="C129" s="4"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C130" s="4"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
+      <c r="B131" t="s">
+        <v>78</v>
+      </c>
       <c r="C131" s="4"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="4"/>
+      <c r="C132" s="4"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>50</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>62</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B145" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>65</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="4" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B154" t="s">
         <v>91</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C154" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="4" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B157" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="4"/>
-      <c r="B157" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="4"/>
+      <c r="B159" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B159" s="4" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C160" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C160" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="C161" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>137</v>
       </c>
-      <c r="B162" s="10" t="s">
+      <c r="B163" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C162" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="C163" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>144</v>
+      </c>
+      <c r="B166" t="s">
         <v>145</v>
       </c>
-      <c r="B165" t="s">
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="B168" t="s">
         <v>147</v>
-      </c>
-      <c r="B167" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>150</v>
-      </c>
-      <c r="C169" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
+        <v>149</v>
+      </c>
+      <c r="C170" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>150</v>
+      </c>
+      <c r="C171" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>151</v>
       </c>
-      <c r="C170" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>152</v>
-      </c>
-      <c r="B172" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>150</v>
-      </c>
-      <c r="C173" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C174" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>150</v>
+      </c>
+      <c r="C175" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>152</v>
+      </c>
+      <c r="B177" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>154</v>
+      </c>
+      <c r="B179" t="s">
+        <v>155</v>
+      </c>
+      <c r="C179" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>156</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>153</v>
       </c>
-      <c r="B176" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>155</v>
-      </c>
-      <c r="B178" t="s">
-        <v>156</v>
-      </c>
-      <c r="C178" t="s">
+      <c r="B182" t="s">
+        <v>158</v>
+      </c>
+      <c r="C182" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>157</v>
-      </c>
-      <c r="C179" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>154</v>
-      </c>
-      <c r="B181" t="s">
-        <v>159</v>
-      </c>
-      <c r="C181" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="B184" t="s">
         <v>164</v>
-      </c>
-      <c r="B183" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>169</v>
+      </c>
+      <c r="B189" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>171</v>
+      </c>
+      <c r="C190" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>170</v>
-      </c>
-      <c r="B188" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
-        <v>172</v>
-      </c>
-      <c r="C189" t="s">
+      <c r="B192" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>169</v>
-      </c>
-      <c r="B191" t="s">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>175</v>
-      </c>
-      <c r="B193" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>180</v>
-      </c>
-      <c r="B198" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>179</v>
+      </c>
+      <c r="B199" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B201" s="4" t="s">
-        <v>183</v>
+      <c r="B201" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B202" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B203" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B204" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C204" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B206" s="4" t="s">
-        <v>206</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B204" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B205" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C205" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B207" t="s">
-        <v>207</v>
-      </c>
-      <c r="C207" t="s">
-        <v>208</v>
+      <c r="B207" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>209</v>
+        <v>206</v>
+      </c>
+      <c r="C208" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B209" s="4" t="s">
-        <v>186</v>
+      <c r="B209" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B210" s="4" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B211" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B212" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>208</v>
+      </c>
+      <c r="C214" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>209</v>
-      </c>
-      <c r="C213" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>130</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B216" t="s">
         <v>131</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C216" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
-        <v>132</v>
-      </c>
-      <c r="C216" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="C217" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>139</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B222" s="4" t="s">
+    <row r="223" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B223" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="330" x14ac:dyDescent="0.25">
-      <c r="B224" s="4" t="s">
-        <v>143</v>
+    <row r="225" spans="2:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="B225" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C179" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
+    <hyperlink ref="C180" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -2840,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD9A0C4-7338-415A-8AC4-B66EAEFEBD21}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2858,7 +2886,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -2877,14 +2905,14 @@
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -2951,7 +2979,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2961,7 +2989,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2976,7 +3004,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3009,17 +3037,17 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3042,7 +3070,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B38" t="s">
         <v>66</v>
@@ -3050,94 +3078,122 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="B45" t="s">
-        <v>197</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>219</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>220</v>
+        <v>269</v>
+      </c>
+      <c r="B53" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>229</v>
-      </c>
       <c r="B55" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3151,7 +3207,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3163,10 +3219,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>256</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -3185,20 +3241,20 @@
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3217,7 +3273,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
         <v>66</v>
@@ -3225,22 +3281,22 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
@@ -3248,7 +3304,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Open CV installation instructions
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003FF156-C559-4A6F-8A2D-DF631EF37076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65975E18-49CD-4F13-833C-3D9E855CA48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="2565" windowWidth="23115" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="7170" yWindow="1860" windowWidth="29985" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="288">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -1156,6 +1156,45 @@
   </si>
   <si>
     <t>change the directory in the second set of "" to show where you have the website set up - i.e. where index.html, etc. are</t>
+  </si>
+  <si>
+    <t>sudo apt-get install build-essential cmake pkg-config</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libjpeg-dev libtiff5-dev libjasper-dev libpng-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libavcodec-dev libavformat-dev libswscale-dev libv4l-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libxvidcore-dev libx264-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libfontconfig1-dev libcairo2-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libgdk-pixbuf2.0-dev libpango1.0-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libgtk2.0-dev libgtk-3-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libatlas-base-dev gfortran</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libhdf5-dev libhdf5-serial-dev libhdf5-103</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libqtgui4 libqtwebkit4 libqt4-test python3-pyqt5</t>
+  </si>
+  <si>
+    <t>sudo apt-get install python3-dev</t>
+  </si>
+  <si>
+    <t>pip3 install opencv-contrib-python==4.1.0.25</t>
+  </si>
+  <si>
+    <t>required for Raspberry Pi, non-Raspberry Pi may be able to use a later version</t>
   </si>
 </sst>
 </file>
@@ -1590,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,1003 +1902,1071 @@
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>286</v>
+      </c>
+      <c r="C70" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B66" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-    </row>
-    <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="B72" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
       <c r="B81" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
       <c r="B82" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-      <c r="B84" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4" t="s">
-        <v>107</v>
+    </row>
+    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
-      <c r="B86" s="4" t="s">
-        <v>108</v>
+      <c r="B86" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
+      <c r="B87" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>79</v>
+      <c r="A88" s="4"/>
+      <c r="B88" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
-      <c r="B89" s="4" t="s">
-        <v>81</v>
+      <c r="B89" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
-      <c r="B90" s="4" t="s">
-        <v>110</v>
+      <c r="B90" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
-      <c r="B91" s="4" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4" t="s">
-        <v>111</v>
+      <c r="A92" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
-      <c r="B93" s="4" t="s">
-        <v>114</v>
+      <c r="B93" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4" t="s">
-        <v>115</v>
+      <c r="B94" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4" t="s">
-        <v>116</v>
+      <c r="B95" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
-      <c r="B96" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C100" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
+      <c r="B99" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="B101" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="C101" s="4"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="C102" s="4"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
-      <c r="B103" t="s">
-        <v>232</v>
-      </c>
-      <c r="C103" s="4"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
-      <c r="B104" t="s">
-        <v>233</v>
-      </c>
-      <c r="C104" s="4"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
-      <c r="B105" t="s">
-        <v>236</v>
-      </c>
-      <c r="C105" s="4"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
-      <c r="B106" t="s">
-        <v>237</v>
-      </c>
-      <c r="C106" s="4"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
-      <c r="B107" t="s">
-        <v>238</v>
-      </c>
-      <c r="C107" s="4"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
-      <c r="B108" t="s">
-        <v>239</v>
-      </c>
-      <c r="C108" s="4"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
-      <c r="B109" t="s">
-        <v>240</v>
-      </c>
-      <c r="C109" s="4"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
-      <c r="B110" t="s">
-        <v>241</v>
-      </c>
-      <c r="C110" s="4"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
-      <c r="B111" t="s">
-        <v>242</v>
-      </c>
-      <c r="C111" s="4"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
-      <c r="B112" t="s">
-        <v>243</v>
-      </c>
-      <c r="C112" s="4"/>
+      <c r="B112" s="4"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
-      <c r="B113" t="s">
-        <v>244</v>
-      </c>
-      <c r="C113" s="4"/>
+      <c r="A113" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C113" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
-      <c r="B114" t="s">
-        <v>245</v>
+      <c r="B114" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="C114" s="4"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
-      <c r="B115" t="s">
-        <v>246</v>
+      <c r="B115" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="C115" s="4"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C119" s="4"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C120" s="4"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C121" s="4"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C122" s="4"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
+      <c r="B123" t="s">
+        <v>241</v>
+      </c>
       <c r="C123" s="4"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>258</v>
+      <c r="A124" s="4"/>
+      <c r="B124" t="s">
+        <v>242</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="C126" s="4"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C127" s="4"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="C128" s="4"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="C129" s="4"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" t="s">
-        <v>77</v>
+        <v>248</v>
       </c>
       <c r="C130" s="4"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" t="s">
-        <v>78</v>
+        <v>249</v>
       </c>
       <c r="C131" s="4"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
+      <c r="B132" t="s">
+        <v>250</v>
+      </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="4"/>
+      <c r="B133" t="s">
+        <v>251</v>
+      </c>
+      <c r="C133" s="4"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="4"/>
+      <c r="B134" t="s">
+        <v>252</v>
+      </c>
+      <c r="C134" s="4"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="4"/>
+      <c r="B135" t="s">
+        <v>253</v>
+      </c>
+      <c r="C135" s="4"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="4"/>
+      <c r="C136" s="4"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C137" s="4"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="4"/>
+      <c r="B138" t="s">
+        <v>259</v>
+      </c>
+      <c r="C138" s="4"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="4"/>
+      <c r="B139" t="s">
+        <v>260</v>
+      </c>
+      <c r="C139" s="4"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
+      <c r="B140" t="s">
+        <v>261</v>
+      </c>
+      <c r="C140" s="4"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
+      <c r="B141" t="s">
+        <v>262</v>
+      </c>
+      <c r="C141" s="4"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
+      <c r="B142" t="s">
+        <v>263</v>
+      </c>
+      <c r="C142" s="4"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+      <c r="B143" t="s">
+        <v>77</v>
+      </c>
+      <c r="C143" s="4"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
+      <c r="B144" t="s">
+        <v>78</v>
+      </c>
+      <c r="C144" s="4"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="4"/>
+      <c r="C145" s="4"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>50</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>62</v>
-      </c>
-      <c r="B145" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>65</v>
-      </c>
       <c r="B149" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>124</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="B154" t="s">
-        <v>91</v>
-      </c>
-      <c r="C154" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B157" t="s">
-        <v>95</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="4"/>
+      <c r="A158" t="s">
+        <v>62</v>
+      </c>
       <c r="B158" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="4"/>
       <c r="B159" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C160" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B161" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C161" s="4" t="s">
-        <v>266</v>
+      <c r="B160" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>65</v>
+      </c>
+      <c r="B162" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>137</v>
-      </c>
-      <c r="B163" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C163" s="11" t="s">
-        <v>159</v>
+      <c r="B163" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B167" t="s">
+        <v>91</v>
+      </c>
+      <c r="C167" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B170" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="4"/>
+      <c r="B171" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="4"/>
+      <c r="B172" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B173" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C173" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>137</v>
+      </c>
+      <c r="B176" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C176" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>144</v>
-      </c>
-      <c r="B166" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>146</v>
-      </c>
-      <c r="B168" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>149</v>
-      </c>
-      <c r="C170" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>150</v>
-      </c>
-      <c r="C171" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>151</v>
-      </c>
-      <c r="B173" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>149</v>
-      </c>
-      <c r="C174" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>150</v>
-      </c>
-      <c r="C175" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>152</v>
-      </c>
-      <c r="B177" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B179" t="s">
-        <v>155</v>
-      </c>
-      <c r="C179" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
-        <v>156</v>
-      </c>
-      <c r="C180" s="9" t="s">
-        <v>157</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>146</v>
+      </c>
+      <c r="B181" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>153</v>
-      </c>
       <c r="B182" t="s">
-        <v>158</v>
-      </c>
-      <c r="C182" t="s">
-        <v>162</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>149</v>
+      </c>
+      <c r="C183" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>163</v>
-      </c>
       <c r="B184" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
-        <v>165</v>
+        <v>150</v>
+      </c>
+      <c r="C184" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>151</v>
+      </c>
       <c r="B186" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>169</v>
-      </c>
-      <c r="B189" t="s">
-        <v>170</v>
+        <v>149</v>
+      </c>
+      <c r="C187" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
+        <v>150</v>
+      </c>
+      <c r="C188" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>152</v>
+      </c>
       <c r="B190" t="s">
-        <v>171</v>
-      </c>
-      <c r="C190" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B192" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>174</v>
-      </c>
-      <c r="B194" t="s">
-        <v>178</v>
+        <v>155</v>
+      </c>
+      <c r="C192" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>156</v>
+      </c>
+      <c r="C193" s="9" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>153</v>
+      </c>
       <c r="B195" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
-        <v>176</v>
+        <v>158</v>
+      </c>
+      <c r="C195" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>163</v>
+      </c>
       <c r="B197" t="s">
-        <v>177</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>179</v>
-      </c>
       <c r="B199" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B202" s="4" t="s">
-        <v>182</v>
+      <c r="A202" t="s">
+        <v>169</v>
+      </c>
+      <c r="B202" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B203" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B204" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B205" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C205" t="s">
-        <v>188</v>
+      <c r="B203" t="s">
+        <v>171</v>
+      </c>
+      <c r="C203" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>168</v>
+      </c>
+      <c r="B205" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B207" s="4" t="s">
-        <v>205</v>
+      <c r="A207" t="s">
+        <v>174</v>
+      </c>
+      <c r="B207" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>206</v>
-      </c>
-      <c r="C208" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B210" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B211" s="4" t="s">
-        <v>209</v>
+      <c r="B210" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B212" s="4" t="s">
-        <v>210</v>
+      <c r="A212" t="s">
+        <v>179</v>
+      </c>
+      <c r="B212" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B213" s="4" t="s">
-        <v>211</v>
+      <c r="B213" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B215" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B216" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B217" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B218" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C218" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B220" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>206</v>
+      </c>
+      <c r="C221" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
         <v>208</v>
       </c>
-      <c r="C214" s="4" t="s">
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B223" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B224" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B225" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B226" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>208</v>
+      </c>
+      <c r="C227" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>130</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B229" t="s">
         <v>131</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C229" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
         <v>132</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C230" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
         <v>139</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B235" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B223" s="4" t="s">
+    <row r="236" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B236" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="225" spans="2:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="B225" s="4" t="s">
+    <row r="238" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+      <c r="B238" s="4" t="s">
         <v>268</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C180" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
+    <hyperlink ref="C193" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
revert to fix pass plots
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65975E18-49CD-4F13-833C-3D9E855CA48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9565A60-617B-4C10-B999-7879049B6F1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="1860" windowWidth="29985" windowHeight="19725" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="18045" yWindow="345" windowWidth="32880" windowHeight="18975" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1123,10 +1117,67 @@
     <t>sudo apt-get install python-matplotlib</t>
   </si>
   <si>
+    <t>Update config</t>
+  </si>
+  <si>
+    <t>cd wxcapture/web/config</t>
+  </si>
+  <si>
+    <t>nano config.json</t>
+  </si>
+  <si>
+    <t>look for the line which includes:</t>
+  </si>
+  <si>
+    <t>"web doc root location": "/home/websites/wxcapture/",</t>
+  </si>
+  <si>
+    <t>change the directory in the second set of "" to show where you have the website set up - i.e. where index.html, etc. are</t>
+  </si>
+  <si>
+    <t>sudo apt-get install build-essential cmake pkg-config</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libjpeg-dev libtiff5-dev libjasper-dev libpng-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libavcodec-dev libavformat-dev libswscale-dev libv4l-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libxvidcore-dev libx264-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libfontconfig1-dev libcairo2-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libgdk-pixbuf2.0-dev libpango1.0-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libgtk2.0-dev libgtk-3-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libatlas-base-dev gfortran</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libhdf5-dev libhdf5-serial-dev libhdf5-103</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libqtgui4 libqtwebkit4 libqt4-test python3-pyqt5</t>
+  </si>
+  <si>
+    <t>sudo apt-get install python3-dev</t>
+  </si>
+  <si>
+    <t>pip3 install opencv-contrib-python==4.1.0.25</t>
+  </si>
+  <si>
+    <t>required for Raspberry Pi, non-Raspberry Pi may be able to use a later version</t>
+  </si>
+  <si>
     <t xml:space="preserve"># run the weather satellite prediction code - v2
 # run at 3 minutes past midnight each night OR after a reboot
-3 0 * * * export DISPLAY=:0.0 &amp;&amp; 3 0 * * * DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
-@reboot DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+3 0 * * *  /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+@reboot  /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
 # update TLE files hourly
 0 * * * *  /home/pi/wxcapture/process/update_tle.py  &gt; /dev/null 2&gt;&amp;1
 # update planets TLE files nightly - 1 minute past midnight
@@ -1138,63 +1189,6 @@
 # Run the config validation script - 1 minute past midnight
 1 0 * * *  /home/pi/wxcapture/process/config.py  &gt; /dev/null 2&gt;&amp;1
 </t>
-  </si>
-  <si>
-    <t>Update config</t>
-  </si>
-  <si>
-    <t>cd wxcapture/web/config</t>
-  </si>
-  <si>
-    <t>nano config.json</t>
-  </si>
-  <si>
-    <t>look for the line which includes:</t>
-  </si>
-  <si>
-    <t>"web doc root location": "/home/websites/wxcapture/",</t>
-  </si>
-  <si>
-    <t>change the directory in the second set of "" to show where you have the website set up - i.e. where index.html, etc. are</t>
-  </si>
-  <si>
-    <t>sudo apt-get install build-essential cmake pkg-config</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libjpeg-dev libtiff5-dev libjasper-dev libpng-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libavcodec-dev libavformat-dev libswscale-dev libv4l-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libxvidcore-dev libx264-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libfontconfig1-dev libcairo2-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libgdk-pixbuf2.0-dev libpango1.0-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libgtk2.0-dev libgtk-3-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libatlas-base-dev gfortran</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libhdf5-dev libhdf5-serial-dev libhdf5-103</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libqtgui4 libqtwebkit4 libqt4-test python3-pyqt5</t>
-  </si>
-  <si>
-    <t>sudo apt-get install python3-dev</t>
-  </si>
-  <si>
-    <t>pip3 install opencv-contrib-python==4.1.0.25</t>
-  </si>
-  <si>
-    <t>required for Raspberry Pi, non-Raspberry Pi may be able to use a later version</t>
   </si>
 </sst>
 </file>
@@ -1631,9 +1625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
   <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1904,57 +1896,57 @@
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
@@ -2004,10 +1996,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>285</v>
+      </c>
+      <c r="C70" t="s">
         <v>286</v>
-      </c>
-      <c r="C70" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2961,7 +2953,7 @@
     </row>
     <row r="238" spans="1:3" ht="375" x14ac:dyDescent="0.25">
       <c r="B238" s="4" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -3251,30 +3243,30 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>268</v>
+      </c>
+      <c r="B53" t="s">
         <v>269</v>
-      </c>
-      <c r="B53" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sync test code and goes17 support
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9565A60-617B-4C10-B999-7879049B6F1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71140E70-05DE-4E37-82B1-FBD96D3C8D99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18045" yWindow="345" windowWidth="32880" windowHeight="18975" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="11280" yWindow="1650" windowWidth="32880" windowHeight="18975" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -1176,8 +1176,8 @@
   <si>
     <t xml:space="preserve"># run the weather satellite prediction code - v2
 # run at 3 minutes past midnight each night OR after a reboot
-3 0 * * *  /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
-@reboot  /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+3 0 * * * DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+@reboot DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
 # update TLE files hourly
 0 * * * *  /home/pi/wxcapture/process/update_tle.py  &gt; /dev/null 2&gt;&amp;1
 # update planets TLE files nightly - 1 minute past midnight
@@ -1625,7 +1625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
   <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="B238" sqref="B238"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
New Pi and more GOES 18 changes
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mike\Documents\GitHub\wxcapture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71140E70-05DE-4E37-82B1-FBD96D3C8D99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D23ABB7-E8E8-4BDD-96E9-894A1BD8498D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1650" windowWidth="32880" windowHeight="18975" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="6060" yWindow="870" windowWidth="41145" windowHeight="20880" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Website" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="311">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -131,10 +132,6 @@
     <t>sudo apt-get install rsync</t>
   </si>
   <si>
-    <t>Tested against a Pi 3 running Buster, with the user wxcapture.
-If using a different username, you will need to modify paths, crontab info, etc.</t>
-  </si>
-  <si>
     <t>Make wxcapture user</t>
   </si>
   <si>
@@ -306,12 +303,6 @@
     <t>predict</t>
   </si>
   <si>
-    <t>provide callsign (if any, can leave blank), plus location info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">need to logout / reboot to avoid messed up command line </t>
-  </si>
-  <si>
     <t>wxtoimg setup</t>
   </si>
   <si>
@@ -409,9 +400,6 @@
   </si>
   <si>
     <t>NOTE - the username must be 5 characters or less (predict buffer overflow bug)</t>
-  </si>
-  <si>
-    <t>sudo tar -xvf wxtoimg-linux-armhf-2.11.2-beta.tar -C / ./usr/local</t>
   </si>
   <si>
     <t>rm wxtoimg-linux-armhf-2.11.2-beta.tar</t>
@@ -1083,12 +1071,6 @@
     <t>cd ~/temp</t>
   </si>
   <si>
-    <t>git clone git://github.com/EliasOenal/multimon-ng.git</t>
-  </si>
-  <si>
-    <t>cd multimon-ng</t>
-  </si>
-  <si>
     <t>mkdir build</t>
   </si>
   <si>
@@ -1138,9 +1120,6 @@
     <t>sudo apt-get install build-essential cmake pkg-config</t>
   </si>
   <si>
-    <t>sudo apt-get install libjpeg-dev libtiff5-dev libjasper-dev libpng-dev</t>
-  </si>
-  <si>
     <t>sudo apt-get install libavcodec-dev libavformat-dev libswscale-dev libv4l-dev</t>
   </si>
   <si>
@@ -1162,9 +1141,6 @@
     <t>sudo apt-get install libhdf5-dev libhdf5-serial-dev libhdf5-103</t>
   </si>
   <si>
-    <t>sudo apt-get install libqtgui4 libqtwebkit4 libqt4-test python3-pyqt5</t>
-  </si>
-  <si>
     <t>sudo apt-get install python3-dev</t>
   </si>
   <si>
@@ -1174,28 +1150,126 @@
     <t>required for Raspberry Pi, non-Raspberry Pi may be able to use a later version</t>
   </si>
   <si>
-    <t xml:space="preserve"># run the weather satellite prediction code - v2
+    <t>libjasper-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libjpeg-dev libtiff5-dev libpng-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install  libqtwebkit4 libqt4-test python3-pyqt5</t>
+  </si>
+  <si>
+    <t>libqtgui4</t>
+  </si>
+  <si>
+    <t>https://github.com/ctrlcctrlv/python-atd</t>
+  </si>
+  <si>
+    <t>Code -&gt; Download zip and copy to Pi</t>
+  </si>
+  <si>
+    <t>unzip python-atd-master.zip</t>
+  </si>
+  <si>
+    <t>cd python-atd-master</t>
+  </si>
+  <si>
+    <t>goto the URL below, code, download zip</t>
+  </si>
+  <si>
+    <t>https://github.com/EliasOenal/multimon-ng</t>
+  </si>
+  <si>
+    <t>unzip multimon-ng-master.zip</t>
+  </si>
+  <si>
+    <t>cd multimon-ng-master/</t>
+  </si>
+  <si>
+    <t>sudo apt-get install qt5-qmake</t>
+  </si>
+  <si>
+    <t>sudo apt-get install python3-pip libusb-1.0 cmake libjpeg-progs netpbm sox at libncurses5-dev libncursesw5-dev libjpeg-dev imagemagick libopenjp2-7-dev libpulse-dev libv4l-dev libasound2-dev libgtk-3-dev libfftw3-dev libhamlib-dev pavucontrol qsstv rsync git rtl-sdr build-essential cmake pkg-config libjpeg-dev libtiff5-dev libpng-dev libavcodec-dev libavformat-dev libswscale-dev libv4l-dev libxvidcore-dev libx264-dev libfontconfig1-dev libcairo2-dev libgdk-pixbuf2.0-dev libpango1.0-dev libgtk2.0-dev libgtk-3-dev libatlas-base-dev gfortran libhdf5-dev libhdf5-serial-dev libhdf5-103 python3-pyqt5 python3-dev python3-pip qt5-qmake</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libqtwebkit4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo apt-get install libqt4-test </t>
+  </si>
+  <si>
+    <t>sudo apt-get install libjasper-dev</t>
+  </si>
+  <si>
+    <t>sudo apt-get install libqtgui4</t>
+  </si>
+  <si>
+    <t>Install predict</t>
+  </si>
+  <si>
+    <t>wget https://www.qsl.net/kd2bd/predict-2.3.0.tar.gz</t>
+  </si>
+  <si>
+    <t>cd predict-2.3.0</t>
+  </si>
+  <si>
+    <t>tar -xvf predict-2.3.0.tar.gz</t>
+  </si>
+  <si>
+    <t>sudo ./configure</t>
+  </si>
+  <si>
+    <t>provide callsign (if any, can leave blank), plus location info ( -37.000  174.8 15 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may need to logout / reboot to avoid messed up command line </t>
+  </si>
+  <si>
+    <t>sudo ln -s /usr/local/bin/predict /usr/bin/predict</t>
+  </si>
+  <si>
+    <t># run the weather satellite prediction code - v2
 # run at 3 minutes past midnight each night OR after a reboot
-3 0 * * * DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
-@reboot DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+# 3 0 * * * DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+# @reboot DISPLAY=localhost:0.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+3 0 * * * /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
+@reboot /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
 # update TLE files hourly
-0 * * * *  /home/pi/wxcapture/process/update_tle.py  &gt; /dev/null 2&gt;&amp;1
+0 * * * *  /home/pi/wxcapture/process/update_tle.py &gt; /dev/null 2&gt;&amp;1
 # update planets TLE files nightly - 1 minute past midnight
-1 0 * * *  /home/pi/wxcapture/process/update_planets_tle.py  &gt; /dev/null 2&gt;&amp;1
+1 0 * * *  /home/pi/wxcapture/process/update_planets_tle.py &gt; /dev/null 2&gt;&amp;1
 # update Satellite Status - 1 minute past midnight
 1 0 * * *  /home/pi/wxcapture/process/satellite_status.py  &gt; /dev/null 2&gt;&amp;1
 # Run the file sync script every 2 minutes on every odd minute
 1-59/2 * * * * /home/pi/wxcapture/process/sync.py &gt; /dev/null 2&gt;&amp;1
 # Run the config validation script - 1 minute past midnight
-1 0 * * *  /home/pi/wxcapture/process/config.py  &gt; /dev/null 2&gt;&amp;1
-</t>
+1 0 * * *  /home/pi/wxcapture/process/config.py &gt; /dev/null 2&gt;&amp;1
+# Run the config validation script - 1 minute past midnight
+59 23 * * *  /home/pi/wxcapture/process/yesterday.py &gt; /dev/null 2&gt;&amp;1</t>
+  </si>
+  <si>
+    <t>sudo tar -xvf wxtoimg-linux-armhf-2.11.2-beta.tar -C / ./usr/</t>
+  </si>
+  <si>
+    <t>Tested against a Pi 3 running Buster, with the user wxcapture.
+Pi 4 - MUST use the 32 bit OS, not the 64 bit.
+If using a different username, you will need to modify paths, crontab info, etc.</t>
+  </si>
+  <si>
+    <t>pip3 install pytz tzlocal pyrtlsdr tweepy discord-webhook skyfield opencv-contrib-python matplotlib numpy --upgrade</t>
+  </si>
+  <si>
+    <t>pip3 install -U discord.py</t>
+  </si>
+  <si>
+    <t>pip3 install -U python-dotenv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1248,6 +1322,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF141414"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1282,7 +1362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1308,6 +1388,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1623,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
-  <dimension ref="A1:C238"/>
+  <dimension ref="A1:D248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="B238" sqref="B238"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,12 +1717,12 @@
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="61.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -1650,10 +1731,10 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -1680,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1708,1262 +1789,1369 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="150.75" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B24" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>309</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>310</v>
+      </c>
+      <c r="C64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>277</v>
+      </c>
+      <c r="D70" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="B72" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>285</v>
-      </c>
-      <c r="C70" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="D73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="D74" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="D75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" t="s">
-        <v>128</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-    </row>
-    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B85" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
+      <c r="B84" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="B86" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
+      <c r="B91" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B92" t="s">
-        <v>79</v>
-      </c>
+      <c r="A92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
+      <c r="A93" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
       <c r="B94" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
       <c r="B96" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
-      <c r="B97" s="4" t="s">
-        <v>106</v>
+      <c r="B97" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
+      <c r="B100" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>79</v>
-      </c>
+      <c r="A101" s="4"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="4"/>
+      <c r="A102" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B102" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
+      <c r="B112" s="4" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C113" t="s">
-        <v>122</v>
-      </c>
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="4"/>
+      <c r="A114" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="B114" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="C114" s="4"/>
+        <v>117</v>
+      </c>
+      <c r="C114" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C115" s="4"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
-      <c r="B116" t="s">
-        <v>232</v>
+      <c r="B116" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C119" s="4"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C120" s="4"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C121" s="4"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C122" s="4"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C123" s="4"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C126" s="4"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C127" s="4"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C128" s="4"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C129" s="4"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C130" s="4"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C131" s="4"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C133" s="4"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C134" s="4"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C135" s="4"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
+      <c r="B136" t="s">
+        <v>249</v>
+      </c>
       <c r="C136" s="4"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>258</v>
-      </c>
+      <c r="A137" s="4"/>
       <c r="C137" s="4"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="4"/>
-      <c r="B138" t="s">
-        <v>259</v>
+      <c r="A138" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="C138" s="4"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" t="s">
-        <v>260</v>
-      </c>
-      <c r="C139" s="4"/>
+        <v>287</v>
+      </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" t="s">
-        <v>261</v>
-      </c>
-      <c r="C140" s="4"/>
+        <v>288</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" t="s">
-        <v>262</v>
-      </c>
-      <c r="C141" s="4"/>
+        <v>289</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" t="s">
-        <v>263</v>
-      </c>
-      <c r="C142" s="4"/>
+        <v>290</v>
+      </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" t="s">
-        <v>77</v>
-      </c>
-      <c r="C143" s="4"/>
+        <v>255</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" t="s">
-        <v>78</v>
-      </c>
-      <c r="C144" s="4"/>
+        <v>256</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
-      <c r="C145" s="4"/>
+      <c r="B145" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>50</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="A146" s="4"/>
+      <c r="B146" t="s">
+        <v>76</v>
+      </c>
+      <c r="C146" s="4"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="4"/>
       <c r="B147" t="s">
-        <v>51</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C147" s="4"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
-        <v>52</v>
-      </c>
+      <c r="A148" s="4"/>
+      <c r="C148" s="4"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>297</v>
+      </c>
       <c r="B149" t="s">
-        <v>53</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C149" s="4"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
       <c r="B150" t="s">
-        <v>54</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C150" s="4"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
       <c r="B151" t="s">
-        <v>55</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="C151" s="4"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
       <c r="B152" t="s">
-        <v>56</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="C152" s="4"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
       <c r="B153" t="s">
-        <v>57</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="C153" s="4"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
-        <v>58</v>
-      </c>
+      <c r="A154" s="4"/>
+      <c r="C154" s="4"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="B155" t="s">
-        <v>59</v>
+        <v>90</v>
+      </c>
+      <c r="C155" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>60</v>
-      </c>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+      <c r="C157" s="4"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>62</v>
-      </c>
-      <c r="B158" t="s">
-        <v>63</v>
+        <v>49</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="B170" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>64</v>
+      </c>
+      <c r="B174" t="s">
         <v>65</v>
       </c>
-      <c r="B162" t="s">
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B167" t="s">
-        <v>91</v>
-      </c>
-      <c r="C167" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B170" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="4"/>
-      <c r="B171" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="4"/>
-      <c r="B172" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B173" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C173" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B174" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C174" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>137</v>
-      </c>
-      <c r="B176" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C176" s="11" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>144</v>
-      </c>
-      <c r="B179" t="s">
-        <v>145</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B180" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>146</v>
-      </c>
+      <c r="A181" s="4"/>
       <c r="B181" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="4"/>
       <c r="B182" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
-        <v>149</v>
+      <c r="B183" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="C183" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
-        <v>150</v>
-      </c>
-      <c r="C184" t="s">
-        <v>160</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B184" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>151</v>
-      </c>
-      <c r="B186" t="s">
-        <v>145</v>
+        <v>133</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C186" s="11" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>149</v>
-      </c>
-      <c r="C187" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
-        <v>150</v>
-      </c>
-      <c r="C188" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>152</v>
-      </c>
-      <c r="B190" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>140</v>
+      </c>
+      <c r="B189" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>142</v>
+      </c>
+      <c r="B191" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>154</v>
-      </c>
       <c r="B192" t="s">
-        <v>155</v>
-      </c>
-      <c r="C192" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
+        <v>145</v>
+      </c>
+      <c r="C193" t="s">
         <v>156</v>
       </c>
-      <c r="C193" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>153</v>
-      </c>
-      <c r="B195" t="s">
-        <v>158</v>
-      </c>
-      <c r="C195" t="s">
-        <v>162</v>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>146</v>
+      </c>
+      <c r="C194" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>147</v>
+      </c>
+      <c r="B196" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>163</v>
-      </c>
       <c r="B197" t="s">
-        <v>164</v>
+        <v>145</v>
+      </c>
+      <c r="C197" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>166</v>
+        <v>146</v>
+      </c>
+      <c r="C198" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>148</v>
+      </c>
       <c r="B200" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B202" t="s">
-        <v>170</v>
+        <v>151</v>
+      </c>
+      <c r="C202" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>171</v>
-      </c>
-      <c r="C203" t="s">
-        <v>172</v>
+        <v>152</v>
+      </c>
+      <c r="C203" s="9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="B205" t="s">
-        <v>173</v>
+        <v>154</v>
+      </c>
+      <c r="C205" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B207" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B212" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
-        <v>181</v>
+        <v>167</v>
+      </c>
+      <c r="C213" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B215" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B216" s="4" t="s">
-        <v>183</v>
+      <c r="A215" t="s">
+        <v>164</v>
+      </c>
+      <c r="B215" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B217" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B218" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C218" t="s">
-        <v>188</v>
+      <c r="A217" t="s">
+        <v>170</v>
+      </c>
+      <c r="B217" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B220" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
-        <v>206</v>
-      </c>
-      <c r="C221" t="s">
-        <v>207</v>
+      <c r="B220" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>175</v>
+      </c>
       <c r="B222" t="s">
-        <v>208</v>
+        <v>78</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B223" s="4" t="s">
-        <v>185</v>
+      <c r="B223" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B224" s="4" t="s">
-        <v>209</v>
+      <c r="B224" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B225" s="4" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B227" t="s">
-        <v>208</v>
-      </c>
-      <c r="C227" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>130</v>
-      </c>
-      <c r="B229" t="s">
-        <v>131</v>
-      </c>
-      <c r="C229" t="s">
-        <v>135</v>
+      <c r="B227" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B228" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C228" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B230" t="s">
-        <v>132</v>
-      </c>
-      <c r="C230" t="s">
-        <v>143</v>
+      <c r="B230" s="4" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>133</v>
+        <v>202</v>
+      </c>
+      <c r="C231" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B233" t="s">
-        <v>136</v>
+      <c r="B233" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B234" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>139</v>
-      </c>
-      <c r="B235" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B235" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B236" s="4" t="s">
-        <v>141</v>
+        <v>207</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="375" x14ac:dyDescent="0.25">
-      <c r="B238" s="4" t="s">
-        <v>287</v>
+        <v>204</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>126</v>
+      </c>
+      <c r="B239" t="s">
+        <v>127</v>
+      </c>
+      <c r="C239" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
+        <v>128</v>
+      </c>
+      <c r="C240" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>135</v>
+      </c>
+      <c r="B245" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B246" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B248" s="4" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C193" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
+    <hyperlink ref="C203" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
+    <hyperlink ref="B149" r:id="rId2" display="https://www.qsl.net/kd2bd/predict-2.3.0.tar.gz" xr:uid="{60543044-0C39-4301-84D9-D4FFE3CE1605}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2987,7 +3175,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -2996,24 +3184,24 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -3075,12 +3263,12 @@
         <v>17</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3090,211 +3278,211 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
         <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B53" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B61" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3320,10 +3508,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -3332,30 +3520,30 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3374,38 +3562,38 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidy to reflect latest dependencies
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Mike\Documents\GitHub\wxcapture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Users\mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D23ABB7-E8E8-4BDD-96E9-894A1BD8498D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0B06D8-4E31-488F-9299-CC567F6408E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="870" windowWidth="41145" windowHeight="20880" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="5355" yWindow="525" windowWidth="23445" windowHeight="21780" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Website" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="266">
   <si>
     <t>WxCapture - Setup Pi</t>
   </si>
@@ -66,69 +65,18 @@
     <t>WxCapture - Setup Server</t>
   </si>
   <si>
-    <t>sudo apt-get install libusb-1.0</t>
-  </si>
-  <si>
-    <t>sudo apt-get install cmake</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libjpeg-progs</t>
-  </si>
-  <si>
-    <t>sudo apt-get install netpbm</t>
-  </si>
-  <si>
     <t>Do upgrades for Pi</t>
   </si>
   <si>
     <t>Install libraries</t>
   </si>
   <si>
-    <t>sudo apt-get install sox</t>
-  </si>
-  <si>
-    <t>sudo apt-get install at</t>
-  </si>
-  <si>
-    <t>sudo apt-get install predict</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libncurses5-dev libncursesw5-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libjpeg-dev</t>
-  </si>
-  <si>
     <t>sudo apt-get install imagemagick</t>
   </si>
   <si>
     <t>sudo apt-get install qt5-default</t>
   </si>
   <si>
-    <t>sudo apt-get install libopenjp2-7-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libpulse-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libv4l-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libasound2-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libgtk-3-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libfftw3-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install pavucontrol</t>
-  </si>
-  <si>
-    <t>sudo apt-get install qsstv</t>
-  </si>
-  <si>
     <t>sudo apt-get install rsync</t>
   </si>
   <si>
@@ -240,24 +188,6 @@
     <t>sudo pip3 install tzlocal</t>
   </si>
   <si>
-    <t>sudo pip3 install pyrtlsdr</t>
-  </si>
-  <si>
-    <t>sudo pip3 install tweepy</t>
-  </si>
-  <si>
-    <t>sudo pip3 install -U discord.py</t>
-  </si>
-  <si>
-    <t>sudo pip3 install -U python-dotenv</t>
-  </si>
-  <si>
-    <t>sudo pip3 install discord-webhook</t>
-  </si>
-  <si>
-    <t>sudo pip3 install skyfield</t>
-  </si>
-  <si>
     <t>make</t>
   </si>
   <si>
@@ -267,24 +197,12 @@
     <t>cd ~</t>
   </si>
   <si>
-    <t>mkdir temp</t>
-  </si>
-  <si>
     <t>cd temp</t>
   </si>
   <si>
-    <t>sudo apt-get install rtl-sdr</t>
-  </si>
-  <si>
     <t>Install python-atd</t>
   </si>
   <si>
-    <t>git clone git://github.com/ctrlcctrlv/python-atd</t>
-  </si>
-  <si>
-    <t>cd python-atd</t>
-  </si>
-  <si>
     <t>sudo python3 setup.py install</t>
   </si>
   <si>
@@ -388,9 +306,6 @@
   </si>
   <si>
     <t>must do from VNC or a terminal app where there is X11 forwarding</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libhamlib-dev</t>
   </si>
   <si>
     <t>sudo cp ~/wxcapture/process/tkclscrd.ttf /usr/local/lib/wx</t>
@@ -1080,9 +995,6 @@
     <t>qmake ../multimon-ng.pro</t>
   </si>
   <si>
-    <t>sudo apt-get install python3-pip</t>
-  </si>
-  <si>
     <t>Only need to do this section if you do not have a pi user already set up</t>
   </si>
   <si>
@@ -1096,9 +1008,6 @@
 Altitude:</t>
   </si>
   <si>
-    <t>sudo apt-get install python-matplotlib</t>
-  </si>
-  <si>
     <t>Update config</t>
   </si>
   <si>
@@ -1117,51 +1026,6 @@
     <t>change the directory in the second set of "" to show where you have the website set up - i.e. where index.html, etc. are</t>
   </si>
   <si>
-    <t>sudo apt-get install build-essential cmake pkg-config</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libavcodec-dev libavformat-dev libswscale-dev libv4l-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libxvidcore-dev libx264-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libfontconfig1-dev libcairo2-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libgdk-pixbuf2.0-dev libpango1.0-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libgtk2.0-dev libgtk-3-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libatlas-base-dev gfortran</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libhdf5-dev libhdf5-serial-dev libhdf5-103</t>
-  </si>
-  <si>
-    <t>sudo apt-get install python3-dev</t>
-  </si>
-  <si>
-    <t>pip3 install opencv-contrib-python==4.1.0.25</t>
-  </si>
-  <si>
-    <t>required for Raspberry Pi, non-Raspberry Pi may be able to use a later version</t>
-  </si>
-  <si>
-    <t>libjasper-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install libjpeg-dev libtiff5-dev libpng-dev</t>
-  </si>
-  <si>
-    <t>sudo apt-get install  libqtwebkit4 libqt4-test python3-pyqt5</t>
-  </si>
-  <si>
-    <t>libqtgui4</t>
-  </si>
-  <si>
     <t>https://github.com/ctrlcctrlv/python-atd</t>
   </si>
   <si>
@@ -1184,9 +1048,6 @@
   </si>
   <si>
     <t>cd multimon-ng-master/</t>
-  </si>
-  <si>
-    <t>sudo apt-get install qt5-qmake</t>
   </si>
   <si>
     <t>sudo apt-get install python3-pip libusb-1.0 cmake libjpeg-progs netpbm sox at libncurses5-dev libncursesw5-dev libjpeg-dev imagemagick libopenjp2-7-dev libpulse-dev libv4l-dev libasound2-dev libgtk-3-dev libfftw3-dev libhamlib-dev pavucontrol qsstv rsync git rtl-sdr build-essential cmake pkg-config libjpeg-dev libtiff5-dev libpng-dev libavcodec-dev libavformat-dev libswscale-dev libv4l-dev libxvidcore-dev libx264-dev libfontconfig1-dev libcairo2-dev libgdk-pixbuf2.0-dev libpango1.0-dev libgtk2.0-dev libgtk-3-dev libatlas-base-dev gfortran libhdf5-dev libhdf5-serial-dev libhdf5-103 python3-pyqt5 python3-dev python3-pip qt5-qmake</t>
@@ -1263,6 +1124,9 @@
   </si>
   <si>
     <t>pip3 install -U python-dotenv</t>
+  </si>
+  <si>
+    <t>These may be needed if you hit issues with dependencies</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
-  <dimension ref="A1:D248"/>
+  <dimension ref="A1:D212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>307</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -1731,10 +1595,10 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -1761,12 +1625,12 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -1789,1366 +1653,1130 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="150.75" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="D24" s="15"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>14</v>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>19</v>
+      <c r="B30" s="4" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="14" t="s">
-        <v>20</v>
+      <c r="B31" s="4" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>263</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>309</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>310</v>
-      </c>
-      <c r="C64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>277</v>
-      </c>
-      <c r="D70" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B72" t="s">
-        <v>283</v>
-      </c>
-      <c r="D72" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
-      <c r="B73" t="s">
-        <v>284</v>
-      </c>
-      <c r="D73" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
-      <c r="B74" t="s">
-        <v>285</v>
-      </c>
-      <c r="D74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
-      <c r="B75" t="s">
-        <v>286</v>
-      </c>
-      <c r="D75" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
-      <c r="B76" t="s">
-        <v>85</v>
-      </c>
-      <c r="D76" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
-      <c r="D77" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" s="4"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C80" s="4"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="C81" s="4"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="C82" s="4"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="C83" s="4"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="C84" s="4"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
-    </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="B85" t="s">
+        <v>206</v>
+      </c>
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
       <c r="B86" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="C86" s="4"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="C87" s="4"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="C88" s="4"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="C89" s="4"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C91" s="4"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="B92" t="s">
+        <v>213</v>
+      </c>
+      <c r="C92" s="4"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
       <c r="B93" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="C93" s="4"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
       <c r="B95" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C95" s="4"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
       <c r="B96" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="C96" s="4"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="C97" s="4"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
-      <c r="B98" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>219</v>
+      </c>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>220</v>
+      </c>
+      <c r="C99" s="4"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
-      <c r="B100" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>221</v>
+      </c>
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101" s="4"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="C102" s="4"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
-      <c r="B103" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
-      <c r="B104" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
-      <c r="B105" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
-      <c r="B106" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
-      <c r="B107" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
-      <c r="B108" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
-      <c r="B109" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
-      <c r="B110" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>53</v>
+      </c>
+      <c r="C110" s="4"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
-      <c r="B111" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>54</v>
+      </c>
+      <c r="C111" s="4"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
-      <c r="B112" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="C112" s="4"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
+      <c r="A113" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B113" t="s">
+        <v>252</v>
+      </c>
+      <c r="C113" s="4"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C114" t="s">
-        <v>119</v>
-      </c>
+      <c r="A114" s="4"/>
+      <c r="B114" t="s">
+        <v>254</v>
+      </c>
+      <c r="C114" s="4"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
-      <c r="B115" s="4" t="s">
-        <v>230</v>
+      <c r="B115" t="s">
+        <v>253</v>
       </c>
       <c r="C115" s="4"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
-      <c r="B116" s="4" t="s">
-        <v>231</v>
+      <c r="B116" t="s">
+        <v>255</v>
       </c>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
-      <c r="B118" t="s">
-        <v>229</v>
-      </c>
       <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="4"/>
+      <c r="A119" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B119" t="s">
-        <v>232</v>
-      </c>
-      <c r="C119" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="C119" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
       <c r="B120" t="s">
-        <v>233</v>
-      </c>
-      <c r="C120" s="4"/>
+        <v>257</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
-      <c r="B121" t="s">
-        <v>234</v>
-      </c>
       <c r="C121" s="4"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="4"/>
-      <c r="B122" t="s">
-        <v>235</v>
-      </c>
-      <c r="C122" s="4"/>
+      <c r="A122" t="s">
+        <v>32</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
       <c r="B123" t="s">
-        <v>236</v>
-      </c>
-      <c r="C123" s="4"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
       <c r="B124" t="s">
-        <v>237</v>
-      </c>
-      <c r="C124" s="4"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
       <c r="B125" t="s">
-        <v>238</v>
-      </c>
-      <c r="C125" s="4"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
       <c r="B126" t="s">
-        <v>239</v>
-      </c>
-      <c r="C126" s="4"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
       <c r="B127" t="s">
-        <v>240</v>
-      </c>
-      <c r="C127" s="4"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
       <c r="B128" t="s">
-        <v>241</v>
-      </c>
-      <c r="C128" s="4"/>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>242</v>
-      </c>
-      <c r="C129" s="4"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>243</v>
-      </c>
-      <c r="C130" s="4"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="4"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>244</v>
-      </c>
-      <c r="C131" s="4"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="4"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>245</v>
-      </c>
-      <c r="C132" s="4"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
-      <c r="B133" t="s">
-        <v>246</v>
-      </c>
-      <c r="C133" s="4"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="4"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>44</v>
+      </c>
       <c r="B134" t="s">
-        <v>247</v>
-      </c>
-      <c r="C134" s="4"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>248</v>
-      </c>
-      <c r="C135" s="4"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="4"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>249</v>
-      </c>
-      <c r="C136" s="4"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="4"/>
-      <c r="C137" s="4"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C138" s="4"/>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="4"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>47</v>
+      </c>
+      <c r="B138" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="4"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="4"/>
-      <c r="B142" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="4"/>
-      <c r="B143" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="4"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="B144" t="s">
-        <v>256</v>
+        <v>65</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
       <c r="B145" t="s">
-        <v>257</v>
+        <v>67</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
       <c r="B146" t="s">
-        <v>76</v>
-      </c>
-      <c r="C146" s="4"/>
+        <v>66</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="4"/>
-      <c r="B147" t="s">
-        <v>77</v>
-      </c>
-      <c r="C147" s="4"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="4"/>
-      <c r="C148" s="4"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B149" t="s">
-        <v>298</v>
-      </c>
-      <c r="C149" s="4"/>
+      <c r="B147" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C147" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="4"/>
-      <c r="B150" t="s">
-        <v>300</v>
-      </c>
-      <c r="C150" s="4"/>
+      <c r="A150" t="s">
+        <v>105</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="4"/>
       <c r="B151" t="s">
-        <v>299</v>
-      </c>
-      <c r="C151" s="4"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="4"/>
-      <c r="B152" t="s">
-        <v>301</v>
-      </c>
-      <c r="C152" s="4"/>
+        <v>116</v>
+      </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="4"/>
+      <c r="A153" t="s">
+        <v>112</v>
+      </c>
       <c r="B153" t="s">
-        <v>304</v>
-      </c>
-      <c r="C153" s="4"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="4"/>
-      <c r="C154" s="4"/>
+        <v>113</v>
+      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="4" t="s">
-        <v>89</v>
+      <c r="A155" t="s">
+        <v>114</v>
       </c>
       <c r="B155" t="s">
-        <v>90</v>
-      </c>
-      <c r="C155" t="s">
-        <v>302</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>303</v>
+        <v>113</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="4"/>
-      <c r="C157" s="4"/>
+      <c r="B157" t="s">
+        <v>117</v>
+      </c>
+      <c r="C157" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>49</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>50</v>
+      <c r="B158" t="s">
+        <v>118</v>
+      </c>
+      <c r="C158" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>119</v>
+      </c>
       <c r="B160" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="C161" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="C162" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>120</v>
+      </c>
       <c r="B164" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>122</v>
+      </c>
       <c r="B166" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="C166" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>61</v>
-      </c>
-      <c r="B170" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>121</v>
+      </c>
+      <c r="B169" t="s">
+        <v>126</v>
+      </c>
+      <c r="C169" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>131</v>
+      </c>
       <c r="B171" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>64</v>
-      </c>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>137</v>
+      </c>
       <c r="B176" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B180" t="s">
-        <v>92</v>
+        <v>139</v>
+      </c>
+      <c r="C177" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>136</v>
+      </c>
+      <c r="B179" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="4"/>
+      <c r="A181" t="s">
+        <v>142</v>
+      </c>
       <c r="B181" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="4"/>
       <c r="B182" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B183" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C183" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B184" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C184" s="4" t="s">
-        <v>260</v>
+      <c r="B183" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>133</v>
-      </c>
-      <c r="B186" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C186" s="11" t="s">
-        <v>155</v>
+        <v>147</v>
+      </c>
+      <c r="B186" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>144</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>140</v>
-      </c>
-      <c r="B189" t="s">
-        <v>141</v>
+      <c r="B189" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B190" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>142</v>
-      </c>
-      <c r="B191" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
-        <v>145</v>
-      </c>
-      <c r="C193" t="s">
+      <c r="B191" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B192" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C192" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B194" t="s">
-        <v>146</v>
-      </c>
-      <c r="C194" t="s">
-        <v>156</v>
+      <c r="B194" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>174</v>
+      </c>
+      <c r="C195" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>147</v>
-      </c>
       <c r="B196" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>145</v>
-      </c>
-      <c r="C197" t="s">
-        <v>156</v>
+      <c r="B197" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>146</v>
-      </c>
-      <c r="C198" t="s">
-        <v>156</v>
+      <c r="B198" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B199" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>148</v>
-      </c>
-      <c r="B200" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>150</v>
-      </c>
-      <c r="B202" t="s">
-        <v>151</v>
-      </c>
-      <c r="C202" t="s">
-        <v>157</v>
+      <c r="B200" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>176</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>98</v>
+      </c>
       <c r="B203" t="s">
-        <v>152</v>
-      </c>
-      <c r="C203" s="9" t="s">
-        <v>153</v>
+        <v>99</v>
+      </c>
+      <c r="C203" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>100</v>
+      </c>
+      <c r="C204" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>149</v>
-      </c>
       <c r="B205" t="s">
-        <v>154</v>
-      </c>
-      <c r="C205" t="s">
-        <v>158</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>159</v>
-      </c>
       <c r="B207" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B208" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>107</v>
+      </c>
       <c r="B209" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>165</v>
-      </c>
-      <c r="B212" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>167</v>
-      </c>
-      <c r="C213" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>164</v>
-      </c>
-      <c r="B215" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>170</v>
-      </c>
-      <c r="B217" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>175</v>
-      </c>
-      <c r="B222" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B225" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B226" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B227" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B228" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C228" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B230" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B231" t="s">
-        <v>202</v>
-      </c>
-      <c r="C231" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B232" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B233" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B234" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B235" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B236" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B237" t="s">
-        <v>204</v>
-      </c>
-      <c r="C237" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>126</v>
-      </c>
-      <c r="B239" t="s">
-        <v>127</v>
-      </c>
-      <c r="C239" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B240" t="s">
-        <v>128</v>
-      </c>
-      <c r="C240" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B241" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B242" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B243" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>135</v>
-      </c>
-      <c r="B245" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="B246" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B247" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B248" s="4" t="s">
-        <v>305</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B210" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B212" s="4" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C203" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
-    <hyperlink ref="B149" r:id="rId2" display="https://www.qsl.net/kd2bd/predict-2.3.0.tar.gz" xr:uid="{60543044-0C39-4301-84D9-D4FFE3CE1605}"/>
+    <hyperlink ref="C167" r:id="rId1" xr:uid="{50DE7997-689D-4633-80DA-55A3C989F636}"/>
+    <hyperlink ref="B113" r:id="rId2" display="https://www.qsl.net/kd2bd/predict-2.3.0.tar.gz" xr:uid="{60543044-0C39-4301-84D9-D4FFE3CE1605}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -3175,7 +2803,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -3184,24 +2812,24 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -3254,235 +2882,235 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B45" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="B53" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="B61" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3508,10 +3136,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -3520,30 +3148,30 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3562,38 +3190,38 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed weather.tle not being fetched
</commit_message>
<xml_diff>
--- a/WxCapture.xlsx
+++ b/WxCapture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Users\mike\Documents\GitHub\wxcapture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0B06D8-4E31-488F-9299-CC567F6408E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013EBB4B-2BF4-4118-BE63-BAF8B202AC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="525" windowWidth="23445" windowHeight="21780" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
+    <workbookView xWindow="11235" yWindow="525" windowWidth="34965" windowHeight="21570" xr2:uid="{C8595ED8-0023-443B-990A-9A4DD8813922}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi" sheetId="1" r:id="rId1"/>
@@ -1089,14 +1089,34 @@
     <t>sudo ln -s /usr/local/bin/predict /usr/bin/predict</t>
   </si>
   <si>
+    <t>sudo tar -xvf wxtoimg-linux-armhf-2.11.2-beta.tar -C / ./usr/</t>
+  </si>
+  <si>
+    <t>Tested against a Pi 3 running Buster, with the user wxcapture.
+Pi 4 - MUST use the 32 bit OS, not the 64 bit.
+If using a different username, you will need to modify paths, crontab info, etc.</t>
+  </si>
+  <si>
+    <t>pip3 install pytz tzlocal pyrtlsdr tweepy discord-webhook skyfield opencv-contrib-python matplotlib numpy --upgrade</t>
+  </si>
+  <si>
+    <t>pip3 install -U discord.py</t>
+  </si>
+  <si>
+    <t>pip3 install -U python-dotenv</t>
+  </si>
+  <si>
+    <t>These may be needed if you hit issues with dependencies</t>
+  </si>
+  <si>
     <t># run the weather satellite prediction code - v2
 # run at 3 minutes past midnight each night OR after a reboot
 # 3 0 * * * DISPLAY=localhost:10.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
 # @reboot DISPLAY=localhost:0.0 /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
 3 0 * * * /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
 @reboot /home/pi/wxcapture/process/schedule_passes.py &gt; /dev/null 2&gt;&amp;1
-# update TLE files hourly
-0 * * * *  /home/pi/wxcapture/process/update_tle.py &gt; /dev/null 2&gt;&amp;1
+# update TLE files every 6 hours
+0 */6 * * *  /home/pi/wxcapture/process/update_tle.py &gt; /dev/null 2&gt;&amp;1
 # update planets TLE files nightly - 1 minute past midnight
 1 0 * * *  /home/pi/wxcapture/process/update_planets_tle.py &gt; /dev/null 2&gt;&amp;1
 # update Satellite Status - 1 minute past midnight
@@ -1107,26 +1127,6 @@
 1 0 * * *  /home/pi/wxcapture/process/config.py &gt; /dev/null 2&gt;&amp;1
 # Run the config validation script - 1 minute past midnight
 59 23 * * *  /home/pi/wxcapture/process/yesterday.py &gt; /dev/null 2&gt;&amp;1</t>
-  </si>
-  <si>
-    <t>sudo tar -xvf wxtoimg-linux-armhf-2.11.2-beta.tar -C / ./usr/</t>
-  </si>
-  <si>
-    <t>Tested against a Pi 3 running Buster, with the user wxcapture.
-Pi 4 - MUST use the 32 bit OS, not the 64 bit.
-If using a different username, you will need to modify paths, crontab info, etc.</t>
-  </si>
-  <si>
-    <t>pip3 install pytz tzlocal pyrtlsdr tweepy discord-webhook skyfield opencv-contrib-python matplotlib numpy --upgrade</t>
-  </si>
-  <si>
-    <t>pip3 install -U discord.py</t>
-  </si>
-  <si>
-    <t>pip3 install -U python-dotenv</t>
-  </si>
-  <si>
-    <t>These may be needed if you hit issues with dependencies</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1247,10 +1247,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1570,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9DEF2B-9547-40D6-9E41-05D28A1C3599}">
   <dimension ref="A1:D212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="B212" sqref="B212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -1720,14 +1716,14 @@
       <c r="B24" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>247</v>
@@ -1758,19 +1754,19 @@
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1834,7 +1830,7 @@
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,7 +2766,7 @@
     </row>
     <row r="212" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B212" s="4" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2787,7 +2783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD9A0C4-7338-415A-8AC4-B66EAEFEBD21}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
@@ -2890,32 +2886,32 @@
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+      <c r="B17" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="B19" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3091,7 +3087,7 @@
       <c r="A59" t="s">
         <v>186</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="12" t="s">
         <v>187</v>
       </c>
     </row>

</xml_diff>